<commit_message>
finish editing input to resident excel for PGY1s
</commit_message>
<xml_diff>
--- a/rotationSchedule_app/management/commands/resident_model.xlsx
+++ b/rotationSchedule_app/management/commands/resident_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29880" windowHeight="19720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28760" windowHeight="19780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,46 +507,46 @@
     <t>Jeffrey Chung (Internal Medicine)</t>
   </si>
   <si>
-    <t>Cardiology</t>
-  </si>
-  <si>
-    <t>Ambulatory Oncology</t>
-  </si>
-  <si>
-    <t>Infectious Disease</t>
-  </si>
-  <si>
     <t>Palliative Care</t>
   </si>
   <si>
-    <t>Rheumatology</t>
-  </si>
-  <si>
-    <t>Endocrine</t>
-  </si>
-  <si>
-    <t>Hematology</t>
-  </si>
-  <si>
-    <t>Allergy/Immunology</t>
-  </si>
-  <si>
-    <t>Gastroenterology</t>
-  </si>
-  <si>
-    <t>Pulmonary</t>
-  </si>
-  <si>
     <t>Nutrition</t>
   </si>
   <si>
-    <t>Oncology</t>
-  </si>
-  <si>
     <t>Renal</t>
   </si>
   <si>
-    <t>Dermatology</t>
+    <t>Heme</t>
+  </si>
+  <si>
+    <t>CARDS ELECTIVE</t>
+  </si>
+  <si>
+    <t>Onc_Amb</t>
+  </si>
+  <si>
+    <t>GI</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Rheum</t>
+  </si>
+  <si>
+    <t>ONC</t>
+  </si>
+  <si>
+    <t>Pulm</t>
+  </si>
+  <si>
+    <t>ENDO</t>
+  </si>
+  <si>
+    <t>All_Imm</t>
+  </si>
+  <si>
+    <t>DERM</t>
   </si>
 </sst>
 </file>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -939,6 +939,8 @@
     <col min="9" max="9" width="21.6640625" customWidth="1"/>
     <col min="10" max="10" width="35" customWidth="1"/>
     <col min="11" max="11" width="32.5" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1047,10 +1049,10 @@
         <v>42371</v>
       </c>
       <c r="L2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -1085,10 +1087,10 @@
         <v>42420</v>
       </c>
       <c r="L3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -1123,10 +1125,10 @@
         <v>42490</v>
       </c>
       <c r="L4" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="M4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1161,10 +1163,10 @@
         <v>42532</v>
       </c>
       <c r="L5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -1199,10 +1201,10 @@
         <v>42518</v>
       </c>
       <c r="L6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M6" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -1237,10 +1239,10 @@
         <v>42392</v>
       </c>
       <c r="L7" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1275,10 +1277,10 @@
         <v>42462</v>
       </c>
       <c r="L8" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M8" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1313,10 +1315,10 @@
         <v>42434</v>
       </c>
       <c r="L9" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1351,10 +1353,10 @@
         <v>42434</v>
       </c>
       <c r="L10" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M10" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1389,10 +1391,10 @@
         <v>42280</v>
       </c>
       <c r="L11" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="M11" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -1427,10 +1429,10 @@
         <v>42448</v>
       </c>
       <c r="L12" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M12" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="W12" t="s">
         <v>155</v>
@@ -1468,10 +1470,10 @@
         <v>42490</v>
       </c>
       <c r="L13" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1506,10 +1508,10 @@
         <v>42532</v>
       </c>
       <c r="L14" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1544,10 +1546,10 @@
         <v>42371</v>
       </c>
       <c r="L15" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -1582,10 +1584,10 @@
         <v>42448</v>
       </c>
       <c r="L16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M16" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -1620,10 +1622,10 @@
         <v>42448</v>
       </c>
       <c r="L17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M17" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -1658,10 +1660,10 @@
         <v>42462</v>
       </c>
       <c r="L18" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="M18" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -1696,10 +1698,10 @@
         <v>42406</v>
       </c>
       <c r="L19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M19" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -1734,10 +1736,10 @@
         <v>42490</v>
       </c>
       <c r="L20" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M20" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -1772,10 +1774,10 @@
         <v>42504</v>
       </c>
       <c r="L21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M21" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -1810,10 +1812,10 @@
         <v>42434</v>
       </c>
       <c r="L22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M22" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -1848,10 +1850,10 @@
         <v>42448</v>
       </c>
       <c r="L23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M23" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -1886,10 +1888,10 @@
         <v>42532</v>
       </c>
       <c r="L24" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M24" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -1924,10 +1926,10 @@
         <v>42308</v>
       </c>
       <c r="L25" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M25" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -1958,7 +1960,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M26" t="s">
         <v>175</v>
@@ -1995,10 +1997,10 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M27" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="W27" t="s">
         <v>157</v>
@@ -2036,10 +2038,10 @@
         <v>42371</v>
       </c>
       <c r="L28" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -2074,10 +2076,10 @@
         <v>42385</v>
       </c>
       <c r="L29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M29" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -2112,10 +2114,10 @@
         <v>42322</v>
       </c>
       <c r="L30" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -2150,10 +2152,10 @@
         <v>42434</v>
       </c>
       <c r="L31" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M31" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="W31" t="s">
         <v>158</v>
@@ -2191,10 +2193,10 @@
         <v>42448</v>
       </c>
       <c r="L32" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="M32" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2229,10 +2231,10 @@
         <v>42336</v>
       </c>
       <c r="L33" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M33" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -2267,10 +2269,10 @@
         <v>42392</v>
       </c>
       <c r="L34" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="M34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2305,10 +2307,10 @@
         <v>42350</v>
       </c>
       <c r="L35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M35" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2343,10 +2345,10 @@
         <v>42462</v>
       </c>
       <c r="L36" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M36" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2381,10 +2383,10 @@
         <v>42434</v>
       </c>
       <c r="L37" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M37" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2419,10 +2421,10 @@
         <v>42308</v>
       </c>
       <c r="L38" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M38" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2457,10 +2459,10 @@
         <v>42322</v>
       </c>
       <c r="L39" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M39" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2495,10 +2497,10 @@
         <v>42371</v>
       </c>
       <c r="L40" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M40" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2565,10 +2567,10 @@
         <v>42294</v>
       </c>
       <c r="L42" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M42" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2603,10 +2605,10 @@
         <v>42476</v>
       </c>
       <c r="L43" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M43" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2641,10 +2643,10 @@
         <v>42280</v>
       </c>
       <c r="L44" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M44" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2679,10 +2681,10 @@
         <v>42392</v>
       </c>
       <c r="L45" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M45" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2717,10 +2719,10 @@
         <v>42518</v>
       </c>
       <c r="L46" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M46" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2755,10 +2757,10 @@
         <v>42434</v>
       </c>
       <c r="L47" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M47" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2793,10 +2795,10 @@
         <v>42532</v>
       </c>
       <c r="L48" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M48" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:23">
@@ -2831,10 +2833,10 @@
         <v>42434</v>
       </c>
       <c r="L49" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:23">
@@ -2869,10 +2871,10 @@
         <v>42518</v>
       </c>
       <c r="L50" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M50" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="W50" t="s">
         <v>159</v>
@@ -2942,10 +2944,10 @@
         <v>42434</v>
       </c>
       <c r="L52" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="M52" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:23">
@@ -2980,10 +2982,10 @@
         <v>42490</v>
       </c>
       <c r="L53" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M53" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:23">
@@ -3014,10 +3016,10 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M54" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="W54" t="s">
         <v>160</v>
@@ -3055,10 +3057,10 @@
         <v>42406</v>
       </c>
       <c r="L55" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M55" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:23">
@@ -3093,10 +3095,10 @@
         <v>42462</v>
       </c>
       <c r="L56" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M56" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:23">
@@ -3131,10 +3133,10 @@
         <v>42392</v>
       </c>
       <c r="L57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M57" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:23">
@@ -3169,10 +3171,10 @@
         <v>42336</v>
       </c>
       <c r="L58" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:23">
@@ -3207,10 +3209,10 @@
         <v>42350</v>
       </c>
       <c r="L59" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M59" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:23">
@@ -3245,10 +3247,10 @@
         <v>42448</v>
       </c>
       <c r="L60" t="s">
+        <v>168</v>
+      </c>
+      <c r="M60" t="s">
         <v>170</v>
-      </c>
-      <c r="M60" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:23">
@@ -3283,10 +3285,10 @@
         <v>42322</v>
       </c>
       <c r="L61" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M61" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:23">
@@ -3321,10 +3323,10 @@
         <v>42406</v>
       </c>
       <c r="L62" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:23">
@@ -3359,10 +3361,10 @@
         <v>42504</v>
       </c>
       <c r="L63" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M63" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:23">
@@ -3397,10 +3399,10 @@
         <v>42322</v>
       </c>
       <c r="L64" t="s">
+        <v>166</v>
+      </c>
+      <c r="M64" t="s">
         <v>162</v>
-      </c>
-      <c r="M64" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:23">
@@ -3435,10 +3437,10 @@
         <v>42322</v>
       </c>
       <c r="L65" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M65" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:23">
@@ -3473,10 +3475,10 @@
         <v>42448</v>
       </c>
       <c r="L66" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M66" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="W66" t="s">
         <v>161</v>

</xml_diff>

<commit_message>
state at time of wash u alpha
</commit_message>
<xml_diff>
--- a/rotationSchedule_app/management/commands/resident_model.xlsx
+++ b/rotationSchedule_app/management/commands/resident_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28760" windowHeight="19780" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="283">
   <si>
     <t>Name</t>
   </si>
@@ -547,13 +547,337 @@
   </si>
   <si>
     <t>DERM</t>
+  </si>
+  <si>
+    <t>Amit Bery</t>
+  </si>
+  <si>
+    <t>PGY2</t>
+  </si>
+  <si>
+    <t>Alex Huh</t>
+  </si>
+  <si>
+    <t>Asrar Khan</t>
+  </si>
+  <si>
+    <t>Benjamin Kopecky</t>
+  </si>
+  <si>
+    <t>Ben Rogers</t>
+  </si>
+  <si>
+    <t>Colin Diffie</t>
+  </si>
+  <si>
+    <t>Chris Jones</t>
+  </si>
+  <si>
+    <t>Chien-Jung Lin</t>
+  </si>
+  <si>
+    <t>Catherine McCarthy</t>
+  </si>
+  <si>
+    <t>Connor Woodland</t>
+  </si>
+  <si>
+    <t>Dilan Patel</t>
+  </si>
+  <si>
+    <t>David Pham</t>
+  </si>
+  <si>
+    <t>Derek Yee</t>
+  </si>
+  <si>
+    <t>Danicela Younce</t>
+  </si>
+  <si>
+    <t>Fizza Abbas</t>
+  </si>
+  <si>
+    <t>Farhan Quader</t>
+  </si>
+  <si>
+    <t>Hirak Shah</t>
+  </si>
+  <si>
+    <t>Jaimie Bolda</t>
+  </si>
+  <si>
+    <t>Joseph Brancheck</t>
+  </si>
+  <si>
+    <t>Juan Calix</t>
+  </si>
+  <si>
+    <t>Jason Chan</t>
+  </si>
+  <si>
+    <t>Jacqueline Chen</t>
+  </si>
+  <si>
+    <t>Jeff Friesen</t>
+  </si>
+  <si>
+    <t>Jessica Ma</t>
+  </si>
+  <si>
+    <t>Global Health</t>
+  </si>
+  <si>
+    <t>Justin Maxfield</t>
+  </si>
+  <si>
+    <t>Jonathan Mizrahi</t>
+  </si>
+  <si>
+    <t>Jay Patel</t>
+  </si>
+  <si>
+    <t>Josh Saef</t>
+  </si>
+  <si>
+    <t>Yuan Yuan</t>
+  </si>
+  <si>
+    <t>Lela Ruck</t>
+  </si>
+  <si>
+    <t>Michael Biersmith</t>
+  </si>
+  <si>
+    <t>M. Phillip Fejleh</t>
+  </si>
+  <si>
+    <t>Mate Gergely</t>
+  </si>
+  <si>
+    <t>Milan Kahanda</t>
+  </si>
+  <si>
+    <t>Michael Paley</t>
+  </si>
+  <si>
+    <t>Maanasi Samant</t>
+  </si>
+  <si>
+    <t>Michael Tang</t>
+  </si>
+  <si>
+    <t>Neal Akhave</t>
+  </si>
+  <si>
+    <t>Niall Prendergast</t>
+  </si>
+  <si>
+    <t>Philip Chu</t>
+  </si>
+  <si>
+    <t>Patrick Grierson</t>
+  </si>
+  <si>
+    <t>Peter Yen</t>
+  </si>
+  <si>
+    <t>PGY3</t>
+  </si>
+  <si>
+    <t>Ramzi Abboud</t>
+  </si>
+  <si>
+    <t>Raymond Fohtung</t>
+  </si>
+  <si>
+    <t>Steven Borson</t>
+  </si>
+  <si>
+    <t>Samuel Reinhardt</t>
+  </si>
+  <si>
+    <t>Tanya Devnani</t>
+  </si>
+  <si>
+    <t>Theodore Kim</t>
+  </si>
+  <si>
+    <t>Yeshika Sharma</t>
+  </si>
+  <si>
+    <t>Proc</t>
+  </si>
+  <si>
+    <t>Asthma (WC)</t>
+  </si>
+  <si>
+    <t>QI</t>
+  </si>
+  <si>
+    <t>Underserved</t>
+  </si>
+  <si>
+    <t>Ortho</t>
+  </si>
+  <si>
+    <t>CAER</t>
+  </si>
+  <si>
+    <t>HOSP</t>
+  </si>
+  <si>
+    <t>BMT</t>
+  </si>
+  <si>
+    <t>Adam Fledderman</t>
+  </si>
+  <si>
+    <t>CSTAR</t>
+  </si>
+  <si>
+    <t>Andrew Michelson</t>
+  </si>
+  <si>
+    <t>Amrita Padda</t>
+  </si>
+  <si>
+    <t>VACR (second part)</t>
+  </si>
+  <si>
+    <t>Ashish Rastogi</t>
+  </si>
+  <si>
+    <t>Bahaa Bedair</t>
+  </si>
+  <si>
+    <t>Brittne Halford</t>
+  </si>
+  <si>
+    <t>Brian Pierce</t>
+  </si>
+  <si>
+    <t>VACR</t>
+  </si>
+  <si>
+    <t>Chelsea Pearson</t>
+  </si>
+  <si>
+    <t>Primary Care</t>
+  </si>
+  <si>
+    <t>Christopher Rigell</t>
+  </si>
+  <si>
+    <t>Dmitriy Breytman</t>
+  </si>
+  <si>
+    <t>Emily Steiner</t>
+  </si>
+  <si>
+    <t>Grant Heberton</t>
+  </si>
+  <si>
+    <t>Gregory Ratti</t>
+  </si>
+  <si>
+    <t>Happy Thakkar</t>
+  </si>
+  <si>
+    <t>Indra Bole</t>
+  </si>
+  <si>
+    <t>Ian Ross</t>
+  </si>
+  <si>
+    <t>Jonathan Chatzkel</t>
+  </si>
+  <si>
+    <t>Jesus Jimenez</t>
+  </si>
+  <si>
+    <t>Justin Sheehy</t>
+  </si>
+  <si>
+    <t>Keerthi Karamched</t>
+  </si>
+  <si>
+    <t>Kiran Mahmood</t>
+  </si>
+  <si>
+    <t>Khoan Vu</t>
+  </si>
+  <si>
+    <t>Lauren Levine</t>
+  </si>
+  <si>
+    <t>Li Zhou</t>
+  </si>
+  <si>
+    <t>Melissa DeFoe</t>
+  </si>
+  <si>
+    <t>Meghan Heberton</t>
+  </si>
+  <si>
+    <t>Michael Hesseler</t>
+  </si>
+  <si>
+    <t>Michael Weaver</t>
+  </si>
+  <si>
+    <t>Ningning Ma</t>
+  </si>
+  <si>
+    <t>Nathan Moore</t>
+  </si>
+  <si>
+    <t>Patricia Litkowski</t>
+  </si>
+  <si>
+    <t>Pooja Koolwal</t>
+  </si>
+  <si>
+    <t>Stacy Dai</t>
+  </si>
+  <si>
+    <t>Scott Goldsmith</t>
+  </si>
+  <si>
+    <t>Stephen Hasak</t>
+  </si>
+  <si>
+    <t>Sushma Jonna</t>
+  </si>
+  <si>
+    <t>Scott McHenry</t>
+  </si>
+  <si>
+    <t>Shan Reddy</t>
+  </si>
+  <si>
+    <t>Yevgeniy Khariton</t>
+  </si>
+  <si>
+    <t>Timothy Brian Lumpkin</t>
+  </si>
+  <si>
+    <t>Tokhanh Nguyen</t>
+  </si>
+  <si>
+    <t>Vaiibhav Patel</t>
+  </si>
+  <si>
+    <t>Yosafe Wakwaya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -561,8 +885,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -572,6 +912,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,15 +931,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -923,22 +1274,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X66"/>
+  <dimension ref="A1:X158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="10" max="10" width="35" customWidth="1"/>
-    <col min="11" max="11" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
     <col min="13" max="13" width="25.6640625" customWidth="1"/>
   </cols>
@@ -950,10 +1301,10 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -977,10 +1328,10 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
@@ -1010,7 +1361,7 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="X1" t="s">
@@ -1030,22 +1381,22 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>42295</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>42308</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>42351</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>42364</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>42358</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="2">
         <v>42371</v>
       </c>
       <c r="L2" t="s">
@@ -1068,22 +1419,22 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>42449</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>42462</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>42435</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <v>42448</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <v>42407</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
         <v>42420</v>
       </c>
       <c r="L3" t="s">
@@ -1106,22 +1457,22 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>42491</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>42504</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>42463</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>42476</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
         <v>42477</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="2">
         <v>42490</v>
       </c>
       <c r="L4" t="s">
@@ -1144,22 +1495,22 @@
       <c r="E5" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>42358</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>42371</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>42323</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2">
         <v>42336</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="2">
         <v>42519</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
         <v>42532</v>
       </c>
       <c r="L5" t="s">
@@ -1182,22 +1533,22 @@
       <c r="E6" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>42351</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>42364</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>42519</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="2">
         <v>42532</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
         <v>42505</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="2">
         <v>42518</v>
       </c>
       <c r="L6" t="s">
@@ -1220,22 +1571,22 @@
       <c r="E7" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>42393</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>42406</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>42421</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2">
         <v>42434</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
         <v>42379</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="2">
         <v>42392</v>
       </c>
       <c r="L7" t="s">
@@ -1258,22 +1609,22 @@
       <c r="E8" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>42407</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>42420</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>42421</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>42434</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
         <v>42449</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="2">
         <v>42462</v>
       </c>
       <c r="L8" t="s">
@@ -1296,22 +1647,22 @@
       <c r="E9" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>42358</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>42371</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>42505</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2">
         <v>42518</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
         <v>42421</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="2">
         <v>42434</v>
       </c>
       <c r="L9" t="s">
@@ -1334,22 +1685,22 @@
       <c r="E10" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>42358</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>42371</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>42323</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="2">
         <v>42336</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
         <v>42421</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
         <v>42434</v>
       </c>
       <c r="L10" t="s">
@@ -1372,22 +1723,22 @@
       <c r="E11" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>42358</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>42371</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>42323</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2">
         <v>42336</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
         <v>42267</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
         <v>42280</v>
       </c>
       <c r="L11" t="s">
@@ -1410,22 +1761,22 @@
       <c r="E12" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>42449</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>42462</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>42463</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2">
         <v>42476</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
         <v>42435</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
         <v>42448</v>
       </c>
       <c r="L12" t="s">
@@ -1451,22 +1802,22 @@
       <c r="E13" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>42358</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>42357</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>42449</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="2">
         <v>42462</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="2">
         <v>42477</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="2">
         <v>42490</v>
       </c>
       <c r="L13" t="s">
@@ -1489,22 +1840,22 @@
       <c r="E14" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <v>42351</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>42364</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <v>42372</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="2">
         <v>42385</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="2">
         <v>42519</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
         <v>42532</v>
       </c>
       <c r="L14" t="s">
@@ -1527,22 +1878,22 @@
       <c r="E15" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <v>42393</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>42406</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>42323</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="2">
         <v>42336</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="2">
         <v>42358</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2">
         <v>42371</v>
       </c>
       <c r="L15" t="s">
@@ -1565,22 +1916,22 @@
       <c r="E16" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2">
         <v>42358</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <v>42371</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <v>42323</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="2">
         <v>42336</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="2">
         <v>42435</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2">
         <v>42448</v>
       </c>
       <c r="L16" t="s">
@@ -1603,22 +1954,22 @@
       <c r="E17" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <v>42407</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <v>42420</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <v>42421</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="2">
         <v>42434</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="2">
         <v>42435</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="2">
         <v>42448</v>
       </c>
       <c r="L17" t="s">
@@ -1641,22 +1992,22 @@
       <c r="E18" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="2">
         <v>42358</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <v>42371</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <v>42463</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="2">
         <v>42476</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="2">
         <v>42449</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="2">
         <v>42462</v>
       </c>
       <c r="L18" t="s">
@@ -1679,22 +2030,22 @@
       <c r="E19" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <v>42337</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <v>42350</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <v>42379</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="2">
         <v>42392</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="2">
         <v>42393</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="2">
         <v>42406</v>
       </c>
       <c r="L19" t="s">
@@ -1717,22 +2068,22 @@
       <c r="E20" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <v>42358</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <v>42371</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <v>42351</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="2">
         <v>42364</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="2">
         <v>42477</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="2">
         <v>42490</v>
       </c>
       <c r="L20" t="s">
@@ -1755,22 +2106,22 @@
       <c r="E21" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <v>42358</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <v>42371</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="2">
         <v>42351</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="2">
         <v>42364</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="2">
         <v>42491</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="2">
         <v>42504</v>
       </c>
       <c r="L21" t="s">
@@ -1793,22 +2144,22 @@
       <c r="E22" t="b">
         <v>1</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="2">
         <v>42358</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
         <v>42371</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="2">
         <v>42351</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="2">
         <v>42364</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="2">
         <v>42421</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="2">
         <v>42434</v>
       </c>
       <c r="L22" t="s">
@@ -1831,22 +2182,22 @@
       <c r="E23" t="b">
         <v>1</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="2">
         <v>42358</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2">
         <v>42371</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="2">
         <v>42421</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="2">
         <v>42434</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="2">
         <v>42435</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="2">
         <v>42448</v>
       </c>
       <c r="L23" t="s">
@@ -1869,22 +2220,22 @@
       <c r="E24" t="b">
         <v>1</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="2">
         <v>42267</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="2">
         <v>42280</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="2">
         <v>42449</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="2">
         <v>42462</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="2">
         <v>42519</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="2">
         <v>42532</v>
       </c>
       <c r="L24" t="s">
@@ -1907,22 +2258,22 @@
       <c r="E25" t="b">
         <v>1</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="2">
         <v>42253</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="2">
         <v>42266</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="2">
         <v>42351</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="2">
         <v>42364</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="2">
         <v>42295</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="2">
         <v>42308</v>
       </c>
       <c r="L25" t="s">
@@ -1945,20 +2296,20 @@
       <c r="E26" t="b">
         <v>1</v>
       </c>
-      <c r="F26" s="1">
-        <v>42217</v>
-      </c>
-      <c r="G26" s="1">
+      <c r="F26" s="2">
+        <v>42218</v>
+      </c>
+      <c r="G26" s="2">
         <v>42230</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="2">
         <v>42351</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="2">
         <v>42364</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
       <c r="L26" t="s">
         <v>170</v>
       </c>
@@ -1982,20 +2333,20 @@
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="2">
         <v>42498</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2">
         <v>42510</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="2">
         <v>42491</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="2">
         <v>42504</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
       <c r="L27" t="s">
         <v>165</v>
       </c>
@@ -2019,22 +2370,22 @@
       <c r="E28" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="2">
         <v>42295</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2">
         <v>42308</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="2">
         <v>42309</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="2">
         <v>42322</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="2">
         <v>42358</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="2">
         <v>42371</v>
       </c>
       <c r="L28" t="s">
@@ -2057,22 +2408,22 @@
       <c r="E29" t="b">
         <v>1</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="2">
         <v>42407</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="2">
         <v>42420</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="2">
         <v>42358</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="2">
         <v>42371</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="2">
         <v>42372</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="2">
         <v>42385</v>
       </c>
       <c r="L29" t="s">
@@ -2095,22 +2446,22 @@
       <c r="E30" t="b">
         <v>1</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="2">
         <v>42519</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="2">
         <v>42532</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="2">
         <v>42372</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="2">
         <v>42364</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="2">
         <v>42309</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="2">
         <v>42322</v>
       </c>
       <c r="L30" t="s">
@@ -2133,22 +2484,22 @@
       <c r="E31" t="b">
         <v>1</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="2">
         <v>42449</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="2">
         <v>42462</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="2">
         <v>42435</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31" s="2">
         <v>42448</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="2">
         <v>42421</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="2">
         <v>42434</v>
       </c>
       <c r="L31" t="s">
@@ -2174,22 +2525,22 @@
       <c r="E32" t="b">
         <v>1</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="2">
         <v>42358</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2">
         <v>42371</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="2">
         <v>42421</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32" s="2">
         <v>42434</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="2">
         <v>42435</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="2">
         <v>42448</v>
       </c>
       <c r="L32" t="s">
@@ -2212,22 +2563,22 @@
       <c r="E33" t="b">
         <v>1</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="2">
         <v>42351</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="2">
         <v>42364</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="2">
         <v>42358</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33" s="2">
         <v>42371</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="2">
         <v>42323</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="2">
         <v>42336</v>
       </c>
       <c r="L33" t="s">
@@ -2250,22 +2601,22 @@
       <c r="E34" t="b">
         <v>1</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="2">
         <v>42358</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="2">
         <v>42371</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="2">
         <v>42351</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="2">
         <v>42364</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="2">
         <v>42379</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="2">
         <v>42392</v>
       </c>
       <c r="L34" t="s">
@@ -2288,22 +2639,22 @@
       <c r="E35" t="b">
         <v>1</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="2">
         <v>42351</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="2">
         <v>42364</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="2">
         <v>42358</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="2">
         <v>42371</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35" s="2">
         <v>42337</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="2">
         <v>42350</v>
       </c>
       <c r="L35" t="s">
@@ -2326,22 +2677,22 @@
       <c r="E36" t="b">
         <v>1</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="2">
         <v>42491</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="2">
         <v>42504</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="2">
         <v>42477</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="2">
         <v>42490</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="2">
         <v>42449</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="2">
         <v>42462</v>
       </c>
       <c r="L36" t="s">
@@ -2364,22 +2715,22 @@
       <c r="E37" t="b">
         <v>1</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="2">
         <v>42393</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="2">
         <v>42406</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="2">
         <v>42372</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="2">
         <v>42385</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="2">
         <v>42421</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="2">
         <v>42434</v>
       </c>
       <c r="L37" t="s">
@@ -2402,22 +2753,22 @@
       <c r="E38" t="b">
         <v>1</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="2">
         <v>42477</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="2">
         <v>42490</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="2">
         <v>42491</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="2">
         <v>42504</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="2">
         <v>42295</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="2">
         <v>42308</v>
       </c>
       <c r="L38" t="s">
@@ -2440,22 +2791,22 @@
       <c r="E39" t="b">
         <v>1</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="2">
         <v>42337</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="2">
         <v>42350</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="2">
         <v>42358</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="2">
         <v>42371</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="2">
         <v>42309</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="2">
         <v>42322</v>
       </c>
       <c r="L39" t="s">
@@ -2478,22 +2829,22 @@
       <c r="E40" t="b">
         <v>1</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="2">
         <v>42295</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="2">
         <v>42308</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="2">
         <v>42435</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="2">
         <v>42448</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="2">
         <v>42358</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="2">
         <v>42371</v>
       </c>
       <c r="L40" t="s">
@@ -2516,22 +2867,22 @@
       <c r="E41" t="b">
         <v>1</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="2">
         <v>42358</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="2">
         <v>42371</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="2">
         <v>42372</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="2">
         <v>42027</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J41" s="2">
         <v>42463</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="2">
         <v>42476</v>
       </c>
     </row>
@@ -2548,22 +2899,22 @@
       <c r="E42" t="b">
         <v>1</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="2">
         <v>42358</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="2">
         <v>42371</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="2">
         <v>42351</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42" s="2">
         <v>42364</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J42" s="2">
         <v>42281</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="2">
         <v>42294</v>
       </c>
       <c r="L42" t="s">
@@ -2586,22 +2937,22 @@
       <c r="E43" t="b">
         <v>1</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="2">
         <v>42309</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="2">
         <v>42322</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="2">
         <v>42337</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43" s="2">
         <v>42350</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43" s="2">
         <v>42463</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="2">
         <v>42476</v>
       </c>
       <c r="L43" t="s">
@@ -2624,22 +2975,22 @@
       <c r="E44" t="b">
         <v>1</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="2">
         <v>42393</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="2">
         <v>42406</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44" s="2">
         <v>42407</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44" s="2">
         <v>42420</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44" s="2">
         <v>42267</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="2">
         <v>42280</v>
       </c>
       <c r="L44" t="s">
@@ -2662,22 +3013,22 @@
       <c r="E45" t="b">
         <v>1</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="2">
         <v>42337</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45" s="2">
         <v>42350</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="2">
         <v>42435</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I45" s="2">
         <v>42448</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45" s="2">
         <v>42379</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45" s="2">
         <v>42392</v>
       </c>
       <c r="L45" t="s">
@@ -2700,22 +3051,22 @@
       <c r="E46" t="b">
         <v>1</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="2">
         <v>42351</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="2">
         <v>42364</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="2">
         <v>42323</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46" s="2">
         <v>42336</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46" s="2">
         <v>42505</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="2">
         <v>42518</v>
       </c>
       <c r="L46" t="s">
@@ -2726,7 +3077,7 @@
       </c>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" t="s">
+      <c r="A47" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B47" t="s">
@@ -2738,22 +3089,22 @@
       <c r="E47" t="b">
         <v>1</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="2">
         <v>42281</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="2">
         <v>42294</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="2">
         <v>42295</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47" s="2">
         <v>42308</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47" s="2">
         <v>42421</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47" s="2">
         <v>42434</v>
       </c>
       <c r="L47" t="s">
@@ -2764,7 +3115,7 @@
       </c>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B48" t="s">
@@ -2776,22 +3127,22 @@
       <c r="E48" t="b">
         <v>1</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="2">
         <v>42267</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48" s="2">
         <v>42280</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48" s="2">
         <v>42337</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48" s="2">
         <v>42350</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48" s="2">
         <v>42519</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="2">
         <v>42532</v>
       </c>
       <c r="L48" t="s">
@@ -2802,7 +3153,7 @@
       </c>
     </row>
     <row r="49" spans="1:23">
-      <c r="A49" t="s">
+      <c r="A49" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B49" t="s">
@@ -2814,22 +3165,22 @@
       <c r="E49" t="b">
         <v>1</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="2">
         <v>42239</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="2">
         <v>42252</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H49" s="2">
         <v>42351</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49" s="2">
         <v>42364</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49" s="2">
         <v>42421</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K49" s="2">
         <v>42434</v>
       </c>
       <c r="L49" t="s">
@@ -2840,7 +3191,7 @@
       </c>
     </row>
     <row r="50" spans="1:23">
-      <c r="A50" t="s">
+      <c r="A50" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B50" t="s">
@@ -2852,22 +3203,22 @@
       <c r="E50" t="b">
         <v>1</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="2">
         <v>42358</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="2">
         <v>42371</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50" s="2">
         <v>42519</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50" s="2">
         <v>42532</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J50" s="2">
         <v>42505</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50" s="2">
         <v>42518</v>
       </c>
       <c r="L50" t="s">
@@ -2881,7 +3232,7 @@
       </c>
     </row>
     <row r="51" spans="1:23">
-      <c r="A51" t="s">
+      <c r="A51" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B51" t="s">
@@ -2893,27 +3244,27 @@
       <c r="E51" t="b">
         <v>1</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="2">
         <v>42505</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="2">
         <v>42518</v>
       </c>
-      <c r="H51" s="1">
+      <c r="H51" s="2">
         <v>42477</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51" s="2">
         <v>42490</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J51" s="2">
         <v>42449</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K51" s="2">
         <v>42462</v>
       </c>
     </row>
     <row r="52" spans="1:23">
-      <c r="A52" t="s">
+      <c r="A52" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B52" t="s">
@@ -2925,22 +3276,22 @@
       <c r="E52" t="b">
         <v>1</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="2">
         <v>42323</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G52" s="2">
         <v>42336</v>
       </c>
-      <c r="H52" s="1">
+      <c r="H52" s="2">
         <v>42267</v>
       </c>
-      <c r="I52" s="1">
+      <c r="I52" s="2">
         <v>42280</v>
       </c>
-      <c r="J52" s="1">
+      <c r="J52" s="2">
         <v>42421</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K52" s="2">
         <v>42434</v>
       </c>
       <c r="L52" t="s">
@@ -2951,7 +3302,7 @@
       </c>
     </row>
     <row r="53" spans="1:23">
-      <c r="A53" t="s">
+      <c r="A53" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B53" t="s">
@@ -2963,22 +3314,22 @@
       <c r="E53" t="b">
         <v>1</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53" s="2">
         <v>42323</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G53" s="2">
         <v>42336</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H53" s="2">
         <v>42351</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I53" s="2">
         <v>42364</v>
       </c>
-      <c r="J53" s="1">
+      <c r="J53" s="2">
         <v>42477</v>
       </c>
-      <c r="K53" s="1">
+      <c r="K53" s="2">
         <v>42490</v>
       </c>
       <c r="L53" t="s">
@@ -2989,7 +3340,7 @@
       </c>
     </row>
     <row r="54" spans="1:23">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B54" t="s">
@@ -3001,20 +3352,20 @@
       <c r="E54" t="b">
         <v>1</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F54" s="2">
         <v>42498</v>
       </c>
-      <c r="G54" s="1">
+      <c r="G54" s="2">
         <v>42512</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H54" s="2">
         <v>42491</v>
       </c>
-      <c r="I54" s="1">
+      <c r="I54" s="2">
         <v>42504</v>
       </c>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
       <c r="L54" t="s">
         <v>166</v>
       </c>
@@ -3026,7 +3377,7 @@
       </c>
     </row>
     <row r="55" spans="1:23">
-      <c r="A55" t="s">
+      <c r="A55" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B55" t="s">
@@ -3038,22 +3389,22 @@
       <c r="E55" t="b">
         <v>1</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="2">
         <v>42519</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G55" s="2">
         <v>42532</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H55" s="2">
         <v>42505</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I55" s="2">
         <v>42518</v>
       </c>
-      <c r="J55" s="1">
+      <c r="J55" s="2">
         <v>42393</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K55" s="2">
         <v>42406</v>
       </c>
       <c r="L55" t="s">
@@ -3064,7 +3415,7 @@
       </c>
     </row>
     <row r="56" spans="1:23">
-      <c r="A56" t="s">
+      <c r="A56" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B56" t="s">
@@ -3076,22 +3427,22 @@
       <c r="E56" t="b">
         <v>1</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56" s="2">
         <v>42519</v>
       </c>
-      <c r="G56" s="1">
+      <c r="G56" s="2">
         <v>42532</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H56" s="2">
         <v>42407</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I56" s="2">
         <v>42420</v>
       </c>
-      <c r="J56" s="1">
+      <c r="J56" s="2">
         <v>42449</v>
       </c>
-      <c r="K56" s="1">
+      <c r="K56" s="2">
         <v>42462</v>
       </c>
       <c r="L56" t="s">
@@ -3102,7 +3453,7 @@
       </c>
     </row>
     <row r="57" spans="1:23">
-      <c r="A57" t="s">
+      <c r="A57" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B57" t="s">
@@ -3114,22 +3465,22 @@
       <c r="E57" t="b">
         <v>1</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57" s="2">
         <v>42358</v>
       </c>
-      <c r="G57" s="1">
+      <c r="G57" s="2">
         <v>42371</v>
       </c>
-      <c r="H57" s="1">
+      <c r="H57" s="2">
         <v>42351</v>
       </c>
-      <c r="I57" s="1">
+      <c r="I57" s="2">
         <v>42364</v>
       </c>
-      <c r="J57" s="1">
+      <c r="J57" s="2">
         <v>42379</v>
       </c>
-      <c r="K57" s="1">
+      <c r="K57" s="2">
         <v>42392</v>
       </c>
       <c r="L57" t="s">
@@ -3140,7 +3491,7 @@
       </c>
     </row>
     <row r="58" spans="1:23">
-      <c r="A58" t="s">
+      <c r="A58" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B58" t="s">
@@ -3152,22 +3503,22 @@
       <c r="E58" t="b">
         <v>1</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F58" s="2">
         <v>42435</v>
       </c>
-      <c r="G58" s="1">
+      <c r="G58" s="2">
         <v>42448</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H58" s="2">
         <v>42449</v>
       </c>
-      <c r="I58" s="1">
+      <c r="I58" s="2">
         <v>42462</v>
       </c>
-      <c r="J58" s="1">
+      <c r="J58" s="2">
         <v>42323</v>
       </c>
-      <c r="K58" s="1">
+      <c r="K58" s="2">
         <v>42336</v>
       </c>
       <c r="L58" t="s">
@@ -3178,7 +3529,7 @@
       </c>
     </row>
     <row r="59" spans="1:23">
-      <c r="A59" t="s">
+      <c r="A59" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B59" t="s">
@@ -3190,22 +3541,22 @@
       <c r="E59" t="b">
         <v>1</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="2">
         <v>42491</v>
       </c>
-      <c r="G59" s="1">
+      <c r="G59" s="2">
         <v>42504</v>
       </c>
-      <c r="H59" s="1">
+      <c r="H59" s="2">
         <v>42281</v>
       </c>
-      <c r="I59" s="1">
+      <c r="I59" s="2">
         <v>42294</v>
       </c>
-      <c r="J59" s="1">
+      <c r="J59" s="2">
         <v>42337</v>
       </c>
-      <c r="K59" s="1">
+      <c r="K59" s="2">
         <v>42350</v>
       </c>
       <c r="L59" t="s">
@@ -3216,7 +3567,7 @@
       </c>
     </row>
     <row r="60" spans="1:23">
-      <c r="A60" t="s">
+      <c r="A60" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B60" t="s">
@@ -3228,22 +3579,22 @@
       <c r="E60" t="b">
         <v>1</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60" s="2">
         <v>42358</v>
       </c>
-      <c r="G60" s="1">
+      <c r="G60" s="2">
         <v>42371</v>
       </c>
-      <c r="H60" s="1">
+      <c r="H60" s="2">
         <v>42351</v>
       </c>
-      <c r="I60" s="1">
+      <c r="I60" s="2">
         <v>42364</v>
       </c>
-      <c r="J60" s="1">
+      <c r="J60" s="2">
         <v>42435</v>
       </c>
-      <c r="K60" s="1">
+      <c r="K60" s="2">
         <v>42448</v>
       </c>
       <c r="L60" t="s">
@@ -3254,7 +3605,7 @@
       </c>
     </row>
     <row r="61" spans="1:23">
-      <c r="A61" t="s">
+      <c r="A61" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B61" t="s">
@@ -3266,22 +3617,22 @@
       <c r="E61" t="b">
         <v>1</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="2">
         <v>42463</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G61" s="2">
         <v>42476</v>
       </c>
-      <c r="H61" s="1">
+      <c r="H61" s="2">
         <v>42295</v>
       </c>
-      <c r="I61" s="1">
+      <c r="I61" s="2">
         <v>42308</v>
       </c>
-      <c r="J61" s="1">
+      <c r="J61" s="2">
         <v>42309</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61" s="2">
         <v>42322</v>
       </c>
       <c r="L61" t="s">
@@ -3292,7 +3643,7 @@
       </c>
     </row>
     <row r="62" spans="1:23">
-      <c r="A62" t="s">
+      <c r="A62" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B62" t="s">
@@ -3304,22 +3655,22 @@
       <c r="E62" t="b">
         <v>1</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="2">
         <v>42407</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G62" s="2">
         <v>42420</v>
       </c>
-      <c r="H62" s="1">
+      <c r="H62" s="2">
         <v>42477</v>
       </c>
-      <c r="I62" s="1">
+      <c r="I62" s="2">
         <v>42490</v>
       </c>
-      <c r="J62" s="1">
+      <c r="J62" s="2">
         <v>42393</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K62" s="2">
         <v>42406</v>
       </c>
       <c r="L62" t="s">
@@ -3330,7 +3681,7 @@
       </c>
     </row>
     <row r="63" spans="1:23">
-      <c r="A63" t="s">
+      <c r="A63" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B63" t="s">
@@ -3342,22 +3693,22 @@
       <c r="E63" t="b">
         <v>1</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="2">
         <v>42449</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G63" s="2">
         <v>42462</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H63" s="2">
         <v>42477</v>
       </c>
-      <c r="I63" s="1">
+      <c r="I63" s="2">
         <v>42490</v>
       </c>
-      <c r="J63" s="1">
+      <c r="J63" s="2">
         <v>42491</v>
       </c>
-      <c r="K63" s="1">
+      <c r="K63" s="2">
         <v>42504</v>
       </c>
       <c r="L63" t="s">
@@ -3368,7 +3719,7 @@
       </c>
     </row>
     <row r="64" spans="1:23">
-      <c r="A64" t="s">
+      <c r="A64" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B64" t="s">
@@ -3380,22 +3731,22 @@
       <c r="E64" t="b">
         <v>1</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64" s="2">
         <v>42267</v>
       </c>
-      <c r="G64" s="1">
+      <c r="G64" s="2">
         <v>42280</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H64" s="2">
         <v>42281</v>
       </c>
-      <c r="I64" s="1">
+      <c r="I64" s="2">
         <v>42294</v>
       </c>
-      <c r="J64" s="1">
+      <c r="J64" s="2">
         <v>42309</v>
       </c>
-      <c r="K64" s="1">
+      <c r="K64" s="2">
         <v>42322</v>
       </c>
       <c r="L64" t="s">
@@ -3406,7 +3757,7 @@
       </c>
     </row>
     <row r="65" spans="1:23">
-      <c r="A65" t="s">
+      <c r="A65" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B65" t="s">
@@ -3418,22 +3769,22 @@
       <c r="E65" t="b">
         <v>1</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="2">
         <v>42351</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G65" s="2">
         <v>42364</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H65" s="2">
         <v>42337</v>
       </c>
-      <c r="I65" s="1">
+      <c r="I65" s="2">
         <v>42350</v>
       </c>
-      <c r="J65" s="1">
+      <c r="J65" s="2">
         <v>42309</v>
       </c>
-      <c r="K65" s="1">
+      <c r="K65" s="2">
         <v>42322</v>
       </c>
       <c r="L65" t="s">
@@ -3444,7 +3795,7 @@
       </c>
     </row>
     <row r="66" spans="1:23">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B66" t="s">
@@ -3456,22 +3807,22 @@
       <c r="E66" t="b">
         <v>1</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="2">
         <v>42449</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="2">
         <v>42462</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H66" s="2">
         <v>42463</v>
       </c>
-      <c r="I66" s="1">
+      <c r="I66" s="2">
         <v>42476</v>
       </c>
-      <c r="J66" s="1">
+      <c r="J66" s="2">
         <v>42435</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K66" s="2">
         <v>42448</v>
       </c>
       <c r="L66" t="s">
@@ -3482,6 +3833,1876 @@
       </c>
       <c r="W66" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23">
+      <c r="A67" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" t="s">
+        <v>177</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="L67" t="s">
+        <v>172</v>
+      </c>
+      <c r="M67" t="s">
+        <v>169</v>
+      </c>
+      <c r="N67" t="s">
+        <v>170</v>
+      </c>
+      <c r="O67" t="s">
+        <v>173</v>
+      </c>
+      <c r="P67" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>229</v>
+      </c>
+      <c r="R67" t="s">
+        <v>174</v>
+      </c>
+      <c r="S67" t="s">
+        <v>230</v>
+      </c>
+      <c r="T67" t="s">
+        <v>231</v>
+      </c>
+      <c r="U67" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23">
+      <c r="A68" t="s">
+        <v>178</v>
+      </c>
+      <c r="C68" t="s">
+        <v>177</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+      <c r="L68" t="s">
+        <v>168</v>
+      </c>
+      <c r="M68" t="s">
+        <v>228</v>
+      </c>
+      <c r="N68" t="s">
+        <v>165</v>
+      </c>
+      <c r="O68" t="s">
+        <v>170</v>
+      </c>
+      <c r="P68" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>229</v>
+      </c>
+      <c r="R68" t="s">
+        <v>233</v>
+      </c>
+      <c r="S68" t="s">
+        <v>230</v>
+      </c>
+      <c r="T68" t="s">
+        <v>174</v>
+      </c>
+      <c r="U68" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23">
+      <c r="A69" t="s">
+        <v>179</v>
+      </c>
+      <c r="C69" t="s">
+        <v>177</v>
+      </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
+        <v>166</v>
+      </c>
+      <c r="M69" t="s">
+        <v>166</v>
+      </c>
+      <c r="N69" t="s">
+        <v>228</v>
+      </c>
+      <c r="O69" t="s">
+        <v>164</v>
+      </c>
+      <c r="P69" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>174</v>
+      </c>
+      <c r="R69" t="s">
+        <v>175</v>
+      </c>
+      <c r="S69" t="s">
+        <v>229</v>
+      </c>
+      <c r="T69" t="s">
+        <v>231</v>
+      </c>
+      <c r="U69" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23">
+      <c r="A70" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" t="s">
+        <v>177</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
+        <v>163</v>
+      </c>
+      <c r="M70" t="s">
+        <v>165</v>
+      </c>
+      <c r="N70" t="s">
+        <v>169</v>
+      </c>
+      <c r="O70" t="s">
+        <v>170</v>
+      </c>
+      <c r="P70" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>174</v>
+      </c>
+      <c r="R70" t="s">
+        <v>175</v>
+      </c>
+      <c r="S70" t="s">
+        <v>232</v>
+      </c>
+      <c r="T70" t="s">
+        <v>229</v>
+      </c>
+      <c r="U70" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23">
+      <c r="A71" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" t="s">
+        <v>177</v>
+      </c>
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+      <c r="L71" t="s">
+        <v>166</v>
+      </c>
+      <c r="M71" t="s">
+        <v>168</v>
+      </c>
+      <c r="N71" t="s">
+        <v>172</v>
+      </c>
+      <c r="O71" t="s">
+        <v>170</v>
+      </c>
+      <c r="P71" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>175</v>
+      </c>
+      <c r="R71" t="s">
+        <v>174</v>
+      </c>
+      <c r="S71" t="s">
+        <v>231</v>
+      </c>
+      <c r="T71" t="s">
+        <v>167</v>
+      </c>
+      <c r="U71" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23">
+      <c r="A72" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" t="s">
+        <v>177</v>
+      </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+      <c r="L72" t="s">
+        <v>170</v>
+      </c>
+      <c r="M72" t="s">
+        <v>173</v>
+      </c>
+      <c r="N72" t="s">
+        <v>228</v>
+      </c>
+      <c r="O72" t="s">
+        <v>168</v>
+      </c>
+      <c r="P72" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>229</v>
+      </c>
+      <c r="R72" t="s">
+        <v>167</v>
+      </c>
+      <c r="S72" t="s">
+        <v>174</v>
+      </c>
+      <c r="T72" t="s">
+        <v>233</v>
+      </c>
+      <c r="U72" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23">
+      <c r="A73" t="s">
+        <v>183</v>
+      </c>
+      <c r="C73" t="s">
+        <v>177</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+      <c r="L73" t="s">
+        <v>172</v>
+      </c>
+      <c r="M73" t="s">
+        <v>235</v>
+      </c>
+      <c r="N73" t="s">
+        <v>165</v>
+      </c>
+      <c r="O73" t="s">
+        <v>169</v>
+      </c>
+      <c r="P73" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>167</v>
+      </c>
+      <c r="R73" t="s">
+        <v>167</v>
+      </c>
+      <c r="S73" t="s">
+        <v>229</v>
+      </c>
+      <c r="T73" t="s">
+        <v>229</v>
+      </c>
+      <c r="U73" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23">
+      <c r="A74" t="s">
+        <v>184</v>
+      </c>
+      <c r="C74" t="s">
+        <v>177</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+      <c r="L74" t="s">
+        <v>166</v>
+      </c>
+      <c r="M74" t="s">
+        <v>228</v>
+      </c>
+      <c r="N74" t="s">
+        <v>164</v>
+      </c>
+      <c r="O74" t="s">
+        <v>169</v>
+      </c>
+      <c r="P74" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>232</v>
+      </c>
+      <c r="R74" t="s">
+        <v>167</v>
+      </c>
+      <c r="S74" t="s">
+        <v>174</v>
+      </c>
+      <c r="T74" t="s">
+        <v>175</v>
+      </c>
+      <c r="U74" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23">
+      <c r="A75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" t="s">
+        <v>177</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+      <c r="L75" t="s">
+        <v>173</v>
+      </c>
+      <c r="M75" t="s">
+        <v>164</v>
+      </c>
+      <c r="N75" t="s">
+        <v>163</v>
+      </c>
+      <c r="O75" t="s">
+        <v>165</v>
+      </c>
+      <c r="P75" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>233</v>
+      </c>
+      <c r="R75" t="s">
+        <v>232</v>
+      </c>
+      <c r="S75" t="s">
+        <v>175</v>
+      </c>
+      <c r="T75" t="s">
+        <v>230</v>
+      </c>
+      <c r="U75" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23">
+      <c r="A76" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" t="s">
+        <v>177</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+      <c r="L76" t="s">
+        <v>173</v>
+      </c>
+      <c r="M76" t="s">
+        <v>170</v>
+      </c>
+      <c r="N76" t="s">
+        <v>163</v>
+      </c>
+      <c r="O76" t="s">
+        <v>165</v>
+      </c>
+      <c r="P76" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>229</v>
+      </c>
+      <c r="R76" t="s">
+        <v>230</v>
+      </c>
+      <c r="S76" t="s">
+        <v>232</v>
+      </c>
+      <c r="T76" t="s">
+        <v>167</v>
+      </c>
+      <c r="U76" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23">
+      <c r="A77" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" t="s">
+        <v>177</v>
+      </c>
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+      <c r="L77" t="s">
+        <v>235</v>
+      </c>
+      <c r="M77" t="s">
+        <v>165</v>
+      </c>
+      <c r="N77" t="s">
+        <v>168</v>
+      </c>
+      <c r="O77" t="s">
+        <v>169</v>
+      </c>
+      <c r="P77" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>167</v>
+      </c>
+      <c r="R77" t="s">
+        <v>232</v>
+      </c>
+      <c r="S77" t="s">
+        <v>230</v>
+      </c>
+      <c r="T77" t="s">
+        <v>231</v>
+      </c>
+      <c r="U77" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23">
+      <c r="A78" t="s">
+        <v>188</v>
+      </c>
+      <c r="C78" t="s">
+        <v>177</v>
+      </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+      <c r="L78" t="s">
+        <v>163</v>
+      </c>
+      <c r="M78" t="s">
+        <v>228</v>
+      </c>
+      <c r="N78" t="s">
+        <v>172</v>
+      </c>
+      <c r="O78" t="s">
+        <v>170</v>
+      </c>
+      <c r="P78" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>229</v>
+      </c>
+      <c r="R78" t="s">
+        <v>175</v>
+      </c>
+      <c r="S78" t="s">
+        <v>232</v>
+      </c>
+      <c r="T78" t="s">
+        <v>167</v>
+      </c>
+      <c r="U78" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23">
+      <c r="A79" t="s">
+        <v>189</v>
+      </c>
+      <c r="C79" t="s">
+        <v>177</v>
+      </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+      <c r="L79" t="s">
+        <v>172</v>
+      </c>
+      <c r="M79" t="s">
+        <v>228</v>
+      </c>
+      <c r="N79" t="s">
+        <v>163</v>
+      </c>
+      <c r="O79" t="s">
+        <v>173</v>
+      </c>
+      <c r="P79" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>175</v>
+      </c>
+      <c r="R79" t="s">
+        <v>174</v>
+      </c>
+      <c r="S79" t="s">
+        <v>229</v>
+      </c>
+      <c r="T79" t="s">
+        <v>167</v>
+      </c>
+      <c r="U79" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23">
+      <c r="A80" t="s">
+        <v>190</v>
+      </c>
+      <c r="C80" t="s">
+        <v>177</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+      <c r="L80" t="s">
+        <v>165</v>
+      </c>
+      <c r="M80" t="s">
+        <v>235</v>
+      </c>
+      <c r="N80" t="s">
+        <v>164</v>
+      </c>
+      <c r="O80" t="s">
+        <v>162</v>
+      </c>
+      <c r="P80" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>167</v>
+      </c>
+      <c r="R80" t="s">
+        <v>174</v>
+      </c>
+      <c r="S80" t="s">
+        <v>175</v>
+      </c>
+      <c r="T80" t="s">
+        <v>232</v>
+      </c>
+      <c r="U80" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21">
+      <c r="A81" t="s">
+        <v>191</v>
+      </c>
+      <c r="C81" t="s">
+        <v>177</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+      <c r="L81" t="s">
+        <v>173</v>
+      </c>
+      <c r="M81" t="s">
+        <v>170</v>
+      </c>
+      <c r="N81" t="s">
+        <v>173</v>
+      </c>
+      <c r="O81" t="s">
+        <v>173</v>
+      </c>
+      <c r="P81" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21">
+      <c r="A82" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" t="s">
+        <v>177</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="L82" t="s">
+        <v>168</v>
+      </c>
+      <c r="M82" t="s">
+        <v>164</v>
+      </c>
+      <c r="N82" t="s">
+        <v>228</v>
+      </c>
+      <c r="O82" t="s">
+        <v>165</v>
+      </c>
+      <c r="P82" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>174</v>
+      </c>
+      <c r="R82" t="s">
+        <v>175</v>
+      </c>
+      <c r="S82" t="s">
+        <v>229</v>
+      </c>
+      <c r="T82" t="s">
+        <v>167</v>
+      </c>
+      <c r="U82" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21">
+      <c r="A83" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" t="s">
+        <v>177</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+      <c r="L83" t="s">
+        <v>166</v>
+      </c>
+      <c r="M83" t="s">
+        <v>165</v>
+      </c>
+      <c r="N83" t="s">
+        <v>169</v>
+      </c>
+      <c r="O83" t="s">
+        <v>170</v>
+      </c>
+      <c r="P83" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>175</v>
+      </c>
+      <c r="R83" t="s">
+        <v>174</v>
+      </c>
+      <c r="S83" t="s">
+        <v>167</v>
+      </c>
+      <c r="T83" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21">
+      <c r="A84" t="s">
+        <v>194</v>
+      </c>
+      <c r="C84" t="s">
+        <v>177</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+      <c r="L84" t="s">
+        <v>166</v>
+      </c>
+      <c r="M84" t="s">
+        <v>172</v>
+      </c>
+      <c r="N84" t="s">
+        <v>228</v>
+      </c>
+      <c r="O84" t="s">
+        <v>169</v>
+      </c>
+      <c r="P84" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>229</v>
+      </c>
+      <c r="R84" t="s">
+        <v>174</v>
+      </c>
+      <c r="S84" t="s">
+        <v>175</v>
+      </c>
+      <c r="T84" t="s">
+        <v>232</v>
+      </c>
+      <c r="U84" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21">
+      <c r="A85" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" t="s">
+        <v>177</v>
+      </c>
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+      <c r="L85" t="s">
+        <v>168</v>
+      </c>
+      <c r="M85" t="s">
+        <v>162</v>
+      </c>
+      <c r="N85" t="s">
+        <v>172</v>
+      </c>
+      <c r="O85" t="s">
+        <v>163</v>
+      </c>
+      <c r="P85" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>175</v>
+      </c>
+      <c r="R85" t="s">
+        <v>232</v>
+      </c>
+      <c r="S85" t="s">
+        <v>231</v>
+      </c>
+      <c r="T85" t="s">
+        <v>230</v>
+      </c>
+      <c r="U85" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21">
+      <c r="A86" t="s">
+        <v>196</v>
+      </c>
+      <c r="C86" t="s">
+        <v>177</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="L86" t="s">
+        <v>169</v>
+      </c>
+      <c r="M86" t="s">
+        <v>170</v>
+      </c>
+      <c r="N86" t="s">
+        <v>235</v>
+      </c>
+      <c r="O86" t="s">
+        <v>173</v>
+      </c>
+      <c r="P86" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>174</v>
+      </c>
+      <c r="R86" t="s">
+        <v>231</v>
+      </c>
+      <c r="S86" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21">
+      <c r="A87" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" t="s">
+        <v>177</v>
+      </c>
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+      <c r="L87" t="s">
+        <v>235</v>
+      </c>
+      <c r="M87" t="s">
+        <v>165</v>
+      </c>
+      <c r="N87" t="s">
+        <v>170</v>
+      </c>
+      <c r="O87" t="s">
+        <v>164</v>
+      </c>
+      <c r="P87" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>167</v>
+      </c>
+      <c r="R87" t="s">
+        <v>174</v>
+      </c>
+      <c r="S87" t="s">
+        <v>229</v>
+      </c>
+      <c r="T87" t="s">
+        <v>175</v>
+      </c>
+      <c r="U87" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21">
+      <c r="A88" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" t="s">
+        <v>177</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="L88" t="s">
+        <v>168</v>
+      </c>
+      <c r="M88" t="s">
+        <v>165</v>
+      </c>
+      <c r="N88" t="s">
+        <v>228</v>
+      </c>
+      <c r="O88" t="s">
+        <v>166</v>
+      </c>
+      <c r="P88" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>175</v>
+      </c>
+      <c r="R88" t="s">
+        <v>174</v>
+      </c>
+      <c r="S88" t="s">
+        <v>167</v>
+      </c>
+      <c r="T88" t="s">
+        <v>232</v>
+      </c>
+      <c r="U88" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21">
+      <c r="A89" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C89" t="s">
+        <v>177</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="L89" t="s">
+        <v>172</v>
+      </c>
+      <c r="M89" t="s">
+        <v>164</v>
+      </c>
+      <c r="N89" t="s">
+        <v>162</v>
+      </c>
+      <c r="O89" t="s">
+        <v>168</v>
+      </c>
+      <c r="P89" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>229</v>
+      </c>
+      <c r="R89" t="s">
+        <v>175</v>
+      </c>
+      <c r="S89" t="s">
+        <v>232</v>
+      </c>
+      <c r="T89" t="s">
+        <v>167</v>
+      </c>
+      <c r="U89" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21">
+      <c r="A90" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C90" t="s">
+        <v>177</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="L90" t="s">
+        <v>170</v>
+      </c>
+      <c r="M90" t="s">
+        <v>163</v>
+      </c>
+      <c r="N90" t="s">
+        <v>173</v>
+      </c>
+      <c r="O90" t="s">
+        <v>162</v>
+      </c>
+      <c r="P90" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>232</v>
+      </c>
+      <c r="R90" t="s">
+        <v>230</v>
+      </c>
+      <c r="S90" t="s">
+        <v>231</v>
+      </c>
+      <c r="T90" t="s">
+        <v>174</v>
+      </c>
+      <c r="U90" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21">
+      <c r="A91" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C91" t="s">
+        <v>177</v>
+      </c>
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+      <c r="L91" t="s">
+        <v>169</v>
+      </c>
+      <c r="M91" t="s">
+        <v>235</v>
+      </c>
+      <c r="N91" t="s">
+        <v>173</v>
+      </c>
+      <c r="O91" t="s">
+        <v>166</v>
+      </c>
+      <c r="P91" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>174</v>
+      </c>
+      <c r="R91" t="s">
+        <v>175</v>
+      </c>
+      <c r="S91" t="s">
+        <v>229</v>
+      </c>
+      <c r="T91" t="s">
+        <v>232</v>
+      </c>
+      <c r="U91" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21">
+      <c r="A92" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C92" t="s">
+        <v>177</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+      <c r="L92" t="s">
+        <v>170</v>
+      </c>
+      <c r="M92" t="s">
+        <v>162</v>
+      </c>
+      <c r="N92" t="s">
+        <v>172</v>
+      </c>
+      <c r="O92" t="s">
+        <v>164</v>
+      </c>
+      <c r="P92" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>167</v>
+      </c>
+      <c r="R92" t="s">
+        <v>174</v>
+      </c>
+      <c r="S92" t="s">
+        <v>230</v>
+      </c>
+      <c r="T92" t="s">
+        <v>233</v>
+      </c>
+      <c r="U92" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21">
+      <c r="A93" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C93" t="s">
+        <v>177</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+      <c r="L93" t="s">
+        <v>169</v>
+      </c>
+      <c r="M93" t="s">
+        <v>165</v>
+      </c>
+      <c r="N93" t="s">
+        <v>172</v>
+      </c>
+      <c r="O93" t="s">
+        <v>168</v>
+      </c>
+      <c r="P93" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>175</v>
+      </c>
+      <c r="R93" t="s">
+        <v>229</v>
+      </c>
+      <c r="S93" t="s">
+        <v>167</v>
+      </c>
+      <c r="T93" t="s">
+        <v>174</v>
+      </c>
+      <c r="U93" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21">
+      <c r="A94" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C94" t="s">
+        <v>177</v>
+      </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21">
+      <c r="A95" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C95" t="s">
+        <v>177</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21">
+      <c r="A96" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C96" t="s">
+        <v>177</v>
+      </c>
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C97" t="s">
+        <v>177</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C98" t="s">
+        <v>177</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C99" t="s">
+        <v>177</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C100" t="s">
+        <v>177</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C101" t="s">
+        <v>177</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C102" t="s">
+        <v>177</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C103" t="s">
+        <v>177</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C104" t="s">
+        <v>177</v>
+      </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C106" t="s">
+        <v>177</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C107" t="s">
+        <v>177</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C108" t="s">
+        <v>177</v>
+      </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C109" t="s">
+        <v>177</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C110" t="s">
+        <v>177</v>
+      </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C111" t="s">
+        <v>177</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C112" t="s">
+        <v>177</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19">
+      <c r="A113" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C113" t="s">
+        <v>177</v>
+      </c>
+      <c r="E113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19">
+      <c r="A114" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C114" t="s">
+        <v>177</v>
+      </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19">
+      <c r="A115" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C115" t="s">
+        <v>177</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19">
+      <c r="A116" t="s">
+        <v>236</v>
+      </c>
+      <c r="C116" t="s">
+        <v>220</v>
+      </c>
+      <c r="D116" t="s">
+        <v>237</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+      <c r="L116" t="s">
+        <v>166</v>
+      </c>
+      <c r="M116" t="s">
+        <v>170</v>
+      </c>
+      <c r="N116" t="s">
+        <v>228</v>
+      </c>
+      <c r="O116" t="s">
+        <v>165</v>
+      </c>
+      <c r="P116" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>175</v>
+      </c>
+      <c r="R116" t="s">
+        <v>232</v>
+      </c>
+      <c r="S116" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19">
+      <c r="A117" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" t="s">
+        <v>220</v>
+      </c>
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19">
+      <c r="A118" t="s">
+        <v>239</v>
+      </c>
+      <c r="C118" t="s">
+        <v>220</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19">
+      <c r="A119" t="s">
+        <v>241</v>
+      </c>
+      <c r="C119" t="s">
+        <v>220</v>
+      </c>
+      <c r="D119" t="s">
+        <v>237</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19">
+      <c r="A120" t="s">
+        <v>242</v>
+      </c>
+      <c r="C120" t="s">
+        <v>220</v>
+      </c>
+      <c r="E120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19">
+      <c r="A121" t="s">
+        <v>243</v>
+      </c>
+      <c r="C121" t="s">
+        <v>220</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19">
+      <c r="A122" t="s">
+        <v>244</v>
+      </c>
+      <c r="C122" t="s">
+        <v>220</v>
+      </c>
+      <c r="D122" t="s">
+        <v>245</v>
+      </c>
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19">
+      <c r="A123" t="s">
+        <v>246</v>
+      </c>
+      <c r="C123" t="s">
+        <v>220</v>
+      </c>
+      <c r="D123" t="s">
+        <v>247</v>
+      </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19">
+      <c r="A124" t="s">
+        <v>248</v>
+      </c>
+      <c r="C124" t="s">
+        <v>220</v>
+      </c>
+      <c r="D124" t="s">
+        <v>245</v>
+      </c>
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19">
+      <c r="A125" t="s">
+        <v>249</v>
+      </c>
+      <c r="C125" t="s">
+        <v>220</v>
+      </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19">
+      <c r="A126" t="s">
+        <v>250</v>
+      </c>
+      <c r="C126" t="s">
+        <v>220</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19">
+      <c r="A127" t="s">
+        <v>251</v>
+      </c>
+      <c r="C127" t="s">
+        <v>220</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19">
+      <c r="A128" t="s">
+        <v>252</v>
+      </c>
+      <c r="C128" t="s">
+        <v>220</v>
+      </c>
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>253</v>
+      </c>
+      <c r="C129" t="s">
+        <v>220</v>
+      </c>
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>254</v>
+      </c>
+      <c r="C130" t="s">
+        <v>220</v>
+      </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>255</v>
+      </c>
+      <c r="C131" t="s">
+        <v>220</v>
+      </c>
+      <c r="D131" t="s">
+        <v>201</v>
+      </c>
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>256</v>
+      </c>
+      <c r="C132" t="s">
+        <v>220</v>
+      </c>
+      <c r="E132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>257</v>
+      </c>
+      <c r="C133" t="s">
+        <v>220</v>
+      </c>
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>258</v>
+      </c>
+      <c r="C134" t="s">
+        <v>220</v>
+      </c>
+      <c r="D134" t="s">
+        <v>237</v>
+      </c>
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>259</v>
+      </c>
+      <c r="C135" t="s">
+        <v>220</v>
+      </c>
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C136" t="s">
+        <v>220</v>
+      </c>
+      <c r="D136" t="s">
+        <v>237</v>
+      </c>
+      <c r="E136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C137" t="s">
+        <v>220</v>
+      </c>
+      <c r="E137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C138" t="s">
+        <v>220</v>
+      </c>
+      <c r="D138" t="s">
+        <v>237</v>
+      </c>
+      <c r="E138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C139" t="s">
+        <v>220</v>
+      </c>
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C140" t="s">
+        <v>220</v>
+      </c>
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C141" t="s">
+        <v>220</v>
+      </c>
+      <c r="D141" t="s">
+        <v>237</v>
+      </c>
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C142" t="s">
+        <v>220</v>
+      </c>
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C143" t="s">
+        <v>220</v>
+      </c>
+      <c r="E143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C144" t="s">
+        <v>220</v>
+      </c>
+      <c r="E144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C145" t="s">
+        <v>220</v>
+      </c>
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C146" t="s">
+        <v>220</v>
+      </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C147" t="s">
+        <v>220</v>
+      </c>
+      <c r="D147" t="s">
+        <v>201</v>
+      </c>
+      <c r="E147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C148" t="s">
+        <v>220</v>
+      </c>
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C149" t="s">
+        <v>220</v>
+      </c>
+      <c r="D149" t="s">
+        <v>237</v>
+      </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C150" t="s">
+        <v>220</v>
+      </c>
+      <c r="E150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C151" t="s">
+        <v>220</v>
+      </c>
+      <c r="E151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C152" t="s">
+        <v>220</v>
+      </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C153" t="s">
+        <v>220</v>
+      </c>
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C154" t="s">
+        <v>220</v>
+      </c>
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C155" t="s">
+        <v>220</v>
+      </c>
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C156" t="s">
+        <v>220</v>
+      </c>
+      <c r="E156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C157" t="s">
+        <v>220</v>
+      </c>
+      <c r="E157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C158" t="s">
+        <v>220</v>
+      </c>
+      <c r="D158" t="s">
+        <v>237</v>
+      </c>
+      <c r="E158" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
April 24 state, running tests
have 5block files in management commands file
</commit_message>
<xml_diff>
--- a/rotationSchedule_app/management/commands/resident_model.xlsx
+++ b/rotationSchedule_app/management/commands/resident_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="19760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38260" windowHeight="19700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="292">
   <si>
     <t>Name</t>
   </si>
@@ -868,6 +868,33 @@
   </si>
   <si>
     <t>Yosafe Wakwaya</t>
+  </si>
+  <si>
+    <t>I_Neuro</t>
+  </si>
+  <si>
+    <t>Plotzker</t>
+  </si>
+  <si>
+    <t>Prelim</t>
+  </si>
+  <si>
+    <t>vacationStart4</t>
+  </si>
+  <si>
+    <t>vacationEnd4</t>
+  </si>
+  <si>
+    <t>vacationStart5</t>
+  </si>
+  <si>
+    <t>vacationEnd5</t>
+  </si>
+  <si>
+    <t>vacationStart6</t>
+  </si>
+  <si>
+    <t>vacationEnd6</t>
   </si>
 </sst>
 </file>
@@ -931,8 +958,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -942,9 +975,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1274,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X158"/>
+  <dimension ref="A1:AE167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1292,9 +1331,10 @@
     <col min="11" max="11" width="14.6640625" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
     <col min="13" max="13" width="25.6640625" customWidth="1"/>
+    <col min="26" max="31" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1367,8 +1407,26 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Z1" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>289</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>290</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1405,8 +1463,14 @@
       <c r="M2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1443,8 +1507,14 @@
       <c r="M3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1454,6 +1524,9 @@
       <c r="C4" t="s">
         <v>154</v>
       </c>
+      <c r="D4" t="s">
+        <v>283</v>
+      </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
@@ -1481,8 +1554,14 @@
       <c r="M4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1519,8 +1598,14 @@
       <c r="M5" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1530,6 +1615,9 @@
       <c r="C6" t="s">
         <v>154</v>
       </c>
+      <c r="D6" t="s">
+        <v>283</v>
+      </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
@@ -1557,8 +1645,14 @@
       <c r="M6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1595,8 +1689,14 @@
       <c r="M7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1633,8 +1733,14 @@
       <c r="M8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1671,8 +1777,14 @@
       <c r="M9" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1709,8 +1821,14 @@
       <c r="M10" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1747,8 +1865,14 @@
       <c r="M11" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1788,8 +1912,14 @@
       <c r="W12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1799,6 +1929,9 @@
       <c r="C13" t="s">
         <v>154</v>
       </c>
+      <c r="D13" t="s">
+        <v>283</v>
+      </c>
       <c r="E13" t="b">
         <v>1</v>
       </c>
@@ -1826,8 +1959,14 @@
       <c r="M13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1864,8 +2003,14 @@
       <c r="M14" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1875,6 +2020,9 @@
       <c r="C15" t="s">
         <v>154</v>
       </c>
+      <c r="D15" t="s">
+        <v>283</v>
+      </c>
       <c r="E15" t="b">
         <v>1</v>
       </c>
@@ -1902,8 +2050,14 @@
       <c r="M15" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1940,8 +2094,14 @@
       <c r="M16" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1951,6 +2111,9 @@
       <c r="C17" t="s">
         <v>154</v>
       </c>
+      <c r="D17" t="s">
+        <v>283</v>
+      </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
@@ -1978,8 +2141,14 @@
       <c r="M17" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+    </row>
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -2016,8 +2185,14 @@
       <c r="M18" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -2054,8 +2229,14 @@
       <c r="M19" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2065,6 +2246,9 @@
       <c r="C20" t="s">
         <v>154</v>
       </c>
+      <c r="D20" t="s">
+        <v>283</v>
+      </c>
       <c r="E20" t="b">
         <v>1</v>
       </c>
@@ -2092,8 +2276,14 @@
       <c r="M20" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2130,8 +2320,14 @@
       <c r="M21" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="22" spans="1:23">
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2141,6 +2337,9 @@
       <c r="C22" t="s">
         <v>154</v>
       </c>
+      <c r="D22" t="s">
+        <v>285</v>
+      </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
@@ -2168,8 +2367,14 @@
       <c r="M22" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="23" spans="1:23">
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2206,8 +2411,14 @@
       <c r="M23" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2244,8 +2455,14 @@
       <c r="M24" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="25" spans="1:23">
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2282,8 +2499,14 @@
       <c r="M25" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="26" spans="1:23">
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2292,6 +2515,9 @@
       </c>
       <c r="C26" t="s">
         <v>154</v>
+      </c>
+      <c r="D26" t="s">
+        <v>285</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -2319,8 +2545,14 @@
       <c r="W26" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2356,8 +2588,14 @@
       <c r="W27" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="28" spans="1:23">
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -2394,8 +2632,14 @@
       <c r="M28" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="29" spans="1:23">
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2432,8 +2676,14 @@
       <c r="M29" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="30" spans="1:23">
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2443,6 +2693,9 @@
       <c r="C30" t="s">
         <v>154</v>
       </c>
+      <c r="D30" t="s">
+        <v>285</v>
+      </c>
       <c r="E30" t="b">
         <v>1</v>
       </c>
@@ -2470,8 +2723,14 @@
       <c r="M30" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="31" spans="1:23">
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -2511,8 +2770,14 @@
       <c r="W31" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="32" spans="1:23">
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+    </row>
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2549,8 +2814,14 @@
       <c r="M32" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+    </row>
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2587,8 +2858,14 @@
       <c r="M33" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+    </row>
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -2598,6 +2875,9 @@
       <c r="C34" t="s">
         <v>154</v>
       </c>
+      <c r="D34" t="s">
+        <v>285</v>
+      </c>
       <c r="E34" t="b">
         <v>1</v>
       </c>
@@ -2625,8 +2905,14 @@
       <c r="M34" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+    </row>
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -2663,8 +2949,14 @@
       <c r="M35" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+    </row>
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2701,8 +2993,14 @@
       <c r="M36" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+    </row>
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2739,8 +3037,14 @@
       <c r="M37" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+    </row>
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -2777,8 +3081,14 @@
       <c r="M38" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+    </row>
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -2815,8 +3125,14 @@
       <c r="M39" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+    </row>
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -2853,8 +3169,14 @@
       <c r="M40" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+    </row>
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -2885,8 +3207,14 @@
       <c r="K41" s="2">
         <v>42476</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="2"/>
+    </row>
+    <row r="42" spans="1:31">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -2923,8 +3251,14 @@
       <c r="M42" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+    </row>
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -2961,8 +3295,14 @@
       <c r="M43" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+    </row>
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -2999,8 +3339,14 @@
       <c r="M44" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+    </row>
+    <row r="45" spans="1:31">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -3037,8 +3383,14 @@
       <c r="M45" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+    </row>
+    <row r="46" spans="1:31">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -3075,8 +3427,14 @@
       <c r="M46" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="2"/>
+    </row>
+    <row r="47" spans="1:31">
       <c r="A47" s="3" t="s">
         <v>69</v>
       </c>
@@ -3113,8 +3471,14 @@
       <c r="M47" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+    </row>
+    <row r="48" spans="1:31">
       <c r="A48" s="3" t="s">
         <v>70</v>
       </c>
@@ -3151,8 +3515,14 @@
       <c r="M48" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="49" spans="1:23">
+      <c r="Z48" s="2"/>
+      <c r="AA48" s="2"/>
+      <c r="AB48" s="2"/>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="2"/>
+      <c r="AE48" s="2"/>
+    </row>
+    <row r="49" spans="1:31">
       <c r="A49" s="3" t="s">
         <v>71</v>
       </c>
@@ -3189,8 +3559,14 @@
       <c r="M49" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="50" spans="1:23">
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2"/>
+      <c r="AB49" s="2"/>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+    </row>
+    <row r="50" spans="1:31">
       <c r="A50" s="3" t="s">
         <v>72</v>
       </c>
@@ -3230,8 +3606,14 @@
       <c r="W50" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="51" spans="1:23">
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+    </row>
+    <row r="51" spans="1:31">
       <c r="A51" s="3" t="s">
         <v>73</v>
       </c>
@@ -3262,8 +3644,14 @@
       <c r="K51" s="2">
         <v>42462</v>
       </c>
-    </row>
-    <row r="52" spans="1:23">
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
+      <c r="AB51" s="2"/>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="2"/>
+      <c r="AE51" s="2"/>
+    </row>
+    <row r="52" spans="1:31">
       <c r="A52" s="3" t="s">
         <v>74</v>
       </c>
@@ -3300,8 +3688,14 @@
       <c r="M52" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="53" spans="1:23">
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="2"/>
+      <c r="AE52" s="2"/>
+    </row>
+    <row r="53" spans="1:31">
       <c r="A53" s="3" t="s">
         <v>75</v>
       </c>
@@ -3338,8 +3732,14 @@
       <c r="M53" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="54" spans="1:23">
+      <c r="Z53" s="2"/>
+      <c r="AA53" s="2"/>
+      <c r="AB53" s="2"/>
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="2"/>
+      <c r="AE53" s="2"/>
+    </row>
+    <row r="54" spans="1:31">
       <c r="A54" s="3" t="s">
         <v>76</v>
       </c>
@@ -3375,8 +3775,14 @@
       <c r="W54" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="55" spans="1:23">
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
+      <c r="AB54" s="2"/>
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="2"/>
+      <c r="AE54" s="2"/>
+    </row>
+    <row r="55" spans="1:31">
       <c r="A55" s="3" t="s">
         <v>77</v>
       </c>
@@ -3386,6 +3792,9 @@
       <c r="C55" t="s">
         <v>154</v>
       </c>
+      <c r="D55" t="s">
+        <v>285</v>
+      </c>
       <c r="E55" t="b">
         <v>1</v>
       </c>
@@ -3413,8 +3822,14 @@
       <c r="M55" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="56" spans="1:23">
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
+      <c r="AB55" s="2"/>
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="2"/>
+      <c r="AE55" s="2"/>
+    </row>
+    <row r="56" spans="1:31">
       <c r="A56" s="3" t="s">
         <v>78</v>
       </c>
@@ -3451,8 +3866,14 @@
       <c r="M56" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="57" spans="1:23">
+      <c r="Z56" s="2"/>
+      <c r="AA56" s="2"/>
+      <c r="AB56" s="2"/>
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="2"/>
+      <c r="AE56" s="2"/>
+    </row>
+    <row r="57" spans="1:31">
       <c r="A57" s="3" t="s">
         <v>79</v>
       </c>
@@ -3489,8 +3910,14 @@
       <c r="M57" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="58" spans="1:23">
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
+      <c r="AB57" s="2"/>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="2"/>
+      <c r="AE57" s="2"/>
+    </row>
+    <row r="58" spans="1:31">
       <c r="A58" s="3" t="s">
         <v>80</v>
       </c>
@@ -3527,8 +3954,14 @@
       <c r="M58" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="59" spans="1:23">
+      <c r="Z58" s="2"/>
+      <c r="AA58" s="2"/>
+      <c r="AB58" s="2"/>
+      <c r="AC58" s="2"/>
+      <c r="AD58" s="2"/>
+      <c r="AE58" s="2"/>
+    </row>
+    <row r="59" spans="1:31">
       <c r="A59" s="3" t="s">
         <v>81</v>
       </c>
@@ -3565,8 +3998,14 @@
       <c r="M59" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="60" spans="1:23">
+      <c r="Z59" s="2"/>
+      <c r="AA59" s="2"/>
+      <c r="AB59" s="2"/>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
+      <c r="AE59" s="2"/>
+    </row>
+    <row r="60" spans="1:31">
       <c r="A60" s="3" t="s">
         <v>82</v>
       </c>
@@ -3603,8 +4042,14 @@
       <c r="M60" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="61" spans="1:23">
+      <c r="Z60" s="2"/>
+      <c r="AA60" s="2"/>
+      <c r="AB60" s="2"/>
+      <c r="AC60" s="2"/>
+      <c r="AD60" s="2"/>
+      <c r="AE60" s="2"/>
+    </row>
+    <row r="61" spans="1:31">
       <c r="A61" s="3" t="s">
         <v>83</v>
       </c>
@@ -3641,8 +4086,14 @@
       <c r="M61" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="62" spans="1:23">
+      <c r="Z61" s="2"/>
+      <c r="AA61" s="2"/>
+      <c r="AB61" s="2"/>
+      <c r="AC61" s="2"/>
+      <c r="AD61" s="2"/>
+      <c r="AE61" s="2"/>
+    </row>
+    <row r="62" spans="1:31">
       <c r="A62" s="3" t="s">
         <v>84</v>
       </c>
@@ -3679,8 +4130,14 @@
       <c r="M62" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="63" spans="1:23">
+      <c r="Z62" s="2"/>
+      <c r="AA62" s="2"/>
+      <c r="AB62" s="2"/>
+      <c r="AC62" s="2"/>
+      <c r="AD62" s="2"/>
+      <c r="AE62" s="2"/>
+    </row>
+    <row r="63" spans="1:31">
       <c r="A63" s="3" t="s">
         <v>85</v>
       </c>
@@ -3690,6 +4147,9 @@
       <c r="C63" t="s">
         <v>154</v>
       </c>
+      <c r="D63" t="s">
+        <v>283</v>
+      </c>
       <c r="E63" t="b">
         <v>1</v>
       </c>
@@ -3717,8 +4177,14 @@
       <c r="M63" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="64" spans="1:23">
+      <c r="Z63" s="2"/>
+      <c r="AA63" s="2"/>
+      <c r="AB63" s="2"/>
+      <c r="AC63" s="2"/>
+      <c r="AD63" s="2"/>
+      <c r="AE63" s="2"/>
+    </row>
+    <row r="64" spans="1:31">
       <c r="A64" s="3" t="s">
         <v>86</v>
       </c>
@@ -3728,6 +4194,9 @@
       <c r="C64" t="s">
         <v>154</v>
       </c>
+      <c r="D64" t="s">
+        <v>283</v>
+      </c>
       <c r="E64" t="b">
         <v>1</v>
       </c>
@@ -3755,8 +4224,14 @@
       <c r="M64" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="65" spans="1:23">
+      <c r="Z64" s="2"/>
+      <c r="AA64" s="2"/>
+      <c r="AB64" s="2"/>
+      <c r="AC64" s="2"/>
+      <c r="AD64" s="2"/>
+      <c r="AE64" s="2"/>
+    </row>
+    <row r="65" spans="1:31">
       <c r="A65" s="3" t="s">
         <v>87</v>
       </c>
@@ -3793,8 +4268,14 @@
       <c r="M65" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="66" spans="1:23">
+      <c r="Z65" s="2"/>
+      <c r="AA65" s="2"/>
+      <c r="AB65" s="2"/>
+      <c r="AC65" s="2"/>
+      <c r="AD65" s="2"/>
+      <c r="AE65" s="2"/>
+    </row>
+    <row r="66" spans="1:31">
       <c r="A66" s="3" t="s">
         <v>88</v>
       </c>
@@ -3834,8 +4315,14 @@
       <c r="W66" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="67" spans="1:23">
+      <c r="Z66" s="2"/>
+      <c r="AA66" s="2"/>
+      <c r="AB66" s="2"/>
+      <c r="AC66" s="2"/>
+      <c r="AD66" s="2"/>
+      <c r="AE66" s="2"/>
+    </row>
+    <row r="67" spans="1:31">
       <c r="A67" t="s">
         <v>176</v>
       </c>
@@ -3845,6 +4332,24 @@
       <c r="E67" t="b">
         <v>1</v>
       </c>
+      <c r="F67" s="2">
+        <v>42498</v>
+      </c>
+      <c r="G67" s="2">
+        <v>42511</v>
+      </c>
+      <c r="H67" s="2">
+        <v>42512</v>
+      </c>
+      <c r="I67" s="2">
+        <v>42525</v>
+      </c>
+      <c r="J67" s="2">
+        <v>42456</v>
+      </c>
+      <c r="K67" s="2">
+        <v>42469</v>
+      </c>
       <c r="L67" t="s">
         <v>172</v>
       </c>
@@ -3875,8 +4380,26 @@
       <c r="U67" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="68" spans="1:23">
+      <c r="Z67" s="2">
+        <v>42232</v>
+      </c>
+      <c r="AA67" s="2">
+        <v>42625</v>
+      </c>
+      <c r="AB67" s="2">
+        <v>42288</v>
+      </c>
+      <c r="AC67" s="2">
+        <v>42315</v>
+      </c>
+      <c r="AD67" s="2">
+        <v>42386</v>
+      </c>
+      <c r="AE67" s="2">
+        <v>42413</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31">
       <c r="A68" t="s">
         <v>178</v>
       </c>
@@ -3886,6 +4409,12 @@
       <c r="E68" t="b">
         <v>1</v>
       </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
       <c r="L68" t="s">
         <v>168</v>
       </c>
@@ -3916,8 +4445,14 @@
       <c r="U68" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="69" spans="1:23">
+      <c r="Z68" s="2"/>
+      <c r="AA68" s="2"/>
+      <c r="AB68" s="2"/>
+      <c r="AC68" s="2"/>
+      <c r="AD68" s="2"/>
+      <c r="AE68" s="2"/>
+    </row>
+    <row r="69" spans="1:31">
       <c r="A69" t="s">
         <v>179</v>
       </c>
@@ -3927,6 +4462,12 @@
       <c r="E69" t="b">
         <v>1</v>
       </c>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
       <c r="L69" t="s">
         <v>166</v>
       </c>
@@ -3957,8 +4498,14 @@
       <c r="U69" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="70" spans="1:23">
+      <c r="Z69" s="2"/>
+      <c r="AA69" s="2"/>
+      <c r="AB69" s="2"/>
+      <c r="AC69" s="2"/>
+      <c r="AD69" s="2"/>
+      <c r="AE69" s="2"/>
+    </row>
+    <row r="70" spans="1:31">
       <c r="A70" t="s">
         <v>180</v>
       </c>
@@ -3968,6 +4515,12 @@
       <c r="E70" t="b">
         <v>1</v>
       </c>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
       <c r="L70" t="s">
         <v>163</v>
       </c>
@@ -3998,8 +4551,14 @@
       <c r="U70" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="71" spans="1:23">
+      <c r="Z70" s="2"/>
+      <c r="AA70" s="2"/>
+      <c r="AB70" s="2"/>
+      <c r="AC70" s="2"/>
+      <c r="AD70" s="2"/>
+      <c r="AE70" s="2"/>
+    </row>
+    <row r="71" spans="1:31">
       <c r="A71" t="s">
         <v>181</v>
       </c>
@@ -4009,6 +4568,12 @@
       <c r="E71" t="b">
         <v>1</v>
       </c>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
       <c r="L71" t="s">
         <v>166</v>
       </c>
@@ -4039,8 +4604,14 @@
       <c r="U71" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="72" spans="1:23">
+      <c r="Z71" s="2"/>
+      <c r="AA71" s="2"/>
+      <c r="AB71" s="2"/>
+      <c r="AC71" s="2"/>
+      <c r="AD71" s="2"/>
+      <c r="AE71" s="2"/>
+    </row>
+    <row r="72" spans="1:31">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -4050,6 +4621,12 @@
       <c r="E72" t="b">
         <v>1</v>
       </c>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
       <c r="L72" t="s">
         <v>170</v>
       </c>
@@ -4080,8 +4657,14 @@
       <c r="U72" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="73" spans="1:23">
+      <c r="Z72" s="2"/>
+      <c r="AA72" s="2"/>
+      <c r="AB72" s="2"/>
+      <c r="AC72" s="2"/>
+      <c r="AD72" s="2"/>
+      <c r="AE72" s="2"/>
+    </row>
+    <row r="73" spans="1:31">
       <c r="A73" t="s">
         <v>183</v>
       </c>
@@ -4091,6 +4674,12 @@
       <c r="E73" t="b">
         <v>1</v>
       </c>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
       <c r="L73" t="s">
         <v>172</v>
       </c>
@@ -4121,8 +4710,14 @@
       <c r="U73" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="74" spans="1:23">
+      <c r="Z73" s="2"/>
+      <c r="AA73" s="2"/>
+      <c r="AB73" s="2"/>
+      <c r="AC73" s="2"/>
+      <c r="AD73" s="2"/>
+      <c r="AE73" s="2"/>
+    </row>
+    <row r="74" spans="1:31">
       <c r="A74" t="s">
         <v>184</v>
       </c>
@@ -4132,6 +4727,12 @@
       <c r="E74" t="b">
         <v>1</v>
       </c>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
       <c r="L74" t="s">
         <v>166</v>
       </c>
@@ -4162,8 +4763,14 @@
       <c r="U74" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="75" spans="1:23">
+      <c r="Z74" s="2"/>
+      <c r="AA74" s="2"/>
+      <c r="AB74" s="2"/>
+      <c r="AC74" s="2"/>
+      <c r="AD74" s="2"/>
+      <c r="AE74" s="2"/>
+    </row>
+    <row r="75" spans="1:31">
       <c r="A75" t="s">
         <v>185</v>
       </c>
@@ -4173,6 +4780,12 @@
       <c r="E75" t="b">
         <v>1</v>
       </c>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
       <c r="L75" t="s">
         <v>173</v>
       </c>
@@ -4203,8 +4816,14 @@
       <c r="U75" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="76" spans="1:23">
+      <c r="Z75" s="2"/>
+      <c r="AA75" s="2"/>
+      <c r="AB75" s="2"/>
+      <c r="AC75" s="2"/>
+      <c r="AD75" s="2"/>
+      <c r="AE75" s="2"/>
+    </row>
+    <row r="76" spans="1:31">
       <c r="A76" t="s">
         <v>186</v>
       </c>
@@ -4214,6 +4833,12 @@
       <c r="E76" t="b">
         <v>1</v>
       </c>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
       <c r="L76" t="s">
         <v>173</v>
       </c>
@@ -4244,8 +4869,14 @@
       <c r="U76" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="77" spans="1:23">
+      <c r="Z76" s="2"/>
+      <c r="AA76" s="2"/>
+      <c r="AB76" s="2"/>
+      <c r="AC76" s="2"/>
+      <c r="AD76" s="2"/>
+      <c r="AE76" s="2"/>
+    </row>
+    <row r="77" spans="1:31">
       <c r="A77" t="s">
         <v>187</v>
       </c>
@@ -4255,6 +4886,12 @@
       <c r="E77" t="b">
         <v>1</v>
       </c>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
       <c r="L77" t="s">
         <v>235</v>
       </c>
@@ -4285,8 +4922,14 @@
       <c r="U77" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="78" spans="1:23">
+      <c r="Z77" s="2"/>
+      <c r="AA77" s="2"/>
+      <c r="AB77" s="2"/>
+      <c r="AC77" s="2"/>
+      <c r="AD77" s="2"/>
+      <c r="AE77" s="2"/>
+    </row>
+    <row r="78" spans="1:31">
       <c r="A78" t="s">
         <v>188</v>
       </c>
@@ -4296,6 +4939,12 @@
       <c r="E78" t="b">
         <v>1</v>
       </c>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
       <c r="L78" t="s">
         <v>163</v>
       </c>
@@ -4326,8 +4975,14 @@
       <c r="U78" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="79" spans="1:23">
+      <c r="Z78" s="2"/>
+      <c r="AA78" s="2"/>
+      <c r="AB78" s="2"/>
+      <c r="AC78" s="2"/>
+      <c r="AD78" s="2"/>
+      <c r="AE78" s="2"/>
+    </row>
+    <row r="79" spans="1:31">
       <c r="A79" t="s">
         <v>189</v>
       </c>
@@ -4337,6 +4992,12 @@
       <c r="E79" t="b">
         <v>1</v>
       </c>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
       <c r="L79" t="s">
         <v>172</v>
       </c>
@@ -4367,8 +5028,14 @@
       <c r="U79" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="80" spans="1:23">
+      <c r="Z79" s="2"/>
+      <c r="AA79" s="2"/>
+      <c r="AB79" s="2"/>
+      <c r="AC79" s="2"/>
+      <c r="AD79" s="2"/>
+      <c r="AE79" s="2"/>
+    </row>
+    <row r="80" spans="1:31">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -4378,6 +5045,12 @@
       <c r="E80" t="b">
         <v>1</v>
       </c>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
       <c r="L80" t="s">
         <v>165</v>
       </c>
@@ -4408,8 +5081,14 @@
       <c r="U80" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="81" spans="1:21">
+      <c r="Z80" s="2"/>
+      <c r="AA80" s="2"/>
+      <c r="AB80" s="2"/>
+      <c r="AC80" s="2"/>
+      <c r="AD80" s="2"/>
+      <c r="AE80" s="2"/>
+    </row>
+    <row r="81" spans="1:31">
       <c r="A81" t="s">
         <v>191</v>
       </c>
@@ -4419,6 +5098,12 @@
       <c r="E81" t="b">
         <v>1</v>
       </c>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
       <c r="L81" t="s">
         <v>173</v>
       </c>
@@ -4437,8 +5122,14 @@
       <c r="Q81" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="82" spans="1:21">
+      <c r="Z81" s="2"/>
+      <c r="AA81" s="2"/>
+      <c r="AB81" s="2"/>
+      <c r="AC81" s="2"/>
+      <c r="AD81" s="2"/>
+      <c r="AE81" s="2"/>
+    </row>
+    <row r="82" spans="1:31">
       <c r="A82" t="s">
         <v>192</v>
       </c>
@@ -4448,6 +5139,12 @@
       <c r="E82" t="b">
         <v>1</v>
       </c>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
       <c r="L82" t="s">
         <v>168</v>
       </c>
@@ -4478,8 +5175,14 @@
       <c r="U82" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="83" spans="1:21">
+      <c r="Z82" s="2"/>
+      <c r="AA82" s="2"/>
+      <c r="AB82" s="2"/>
+      <c r="AC82" s="2"/>
+      <c r="AD82" s="2"/>
+      <c r="AE82" s="2"/>
+    </row>
+    <row r="83" spans="1:31">
       <c r="A83" t="s">
         <v>193</v>
       </c>
@@ -4489,6 +5192,12 @@
       <c r="E83" t="b">
         <v>1</v>
       </c>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
       <c r="L83" t="s">
         <v>166</v>
       </c>
@@ -4516,8 +5225,14 @@
       <c r="T83" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="84" spans="1:21">
+      <c r="Z83" s="2"/>
+      <c r="AA83" s="2"/>
+      <c r="AB83" s="2"/>
+      <c r="AC83" s="2"/>
+      <c r="AD83" s="2"/>
+      <c r="AE83" s="2"/>
+    </row>
+    <row r="84" spans="1:31">
       <c r="A84" t="s">
         <v>194</v>
       </c>
@@ -4527,6 +5242,12 @@
       <c r="E84" t="b">
         <v>1</v>
       </c>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
       <c r="L84" t="s">
         <v>166</v>
       </c>
@@ -4557,8 +5278,14 @@
       <c r="U84" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="1:21">
+      <c r="Z84" s="2"/>
+      <c r="AA84" s="2"/>
+      <c r="AB84" s="2"/>
+      <c r="AC84" s="2"/>
+      <c r="AD84" s="2"/>
+      <c r="AE84" s="2"/>
+    </row>
+    <row r="85" spans="1:31">
       <c r="A85" t="s">
         <v>195</v>
       </c>
@@ -4568,6 +5295,12 @@
       <c r="E85" t="b">
         <v>1</v>
       </c>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
       <c r="L85" t="s">
         <v>168</v>
       </c>
@@ -4598,8 +5331,14 @@
       <c r="U85" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="86" spans="1:21">
+      <c r="Z85" s="2"/>
+      <c r="AA85" s="2"/>
+      <c r="AB85" s="2"/>
+      <c r="AC85" s="2"/>
+      <c r="AD85" s="2"/>
+      <c r="AE85" s="2"/>
+    </row>
+    <row r="86" spans="1:31">
       <c r="A86" t="s">
         <v>196</v>
       </c>
@@ -4609,6 +5348,12 @@
       <c r="E86" t="b">
         <v>1</v>
       </c>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
       <c r="L86" t="s">
         <v>169</v>
       </c>
@@ -4633,8 +5378,14 @@
       <c r="S86" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="87" spans="1:21">
+      <c r="Z86" s="2"/>
+      <c r="AA86" s="2"/>
+      <c r="AB86" s="2"/>
+      <c r="AC86" s="2"/>
+      <c r="AD86" s="2"/>
+      <c r="AE86" s="2"/>
+    </row>
+    <row r="87" spans="1:31">
       <c r="A87" s="3" t="s">
         <v>197</v>
       </c>
@@ -4644,6 +5395,12 @@
       <c r="E87" t="b">
         <v>1</v>
       </c>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
       <c r="L87" t="s">
         <v>235</v>
       </c>
@@ -4674,8 +5431,14 @@
       <c r="U87" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="88" spans="1:21">
+      <c r="Z87" s="2"/>
+      <c r="AA87" s="2"/>
+      <c r="AB87" s="2"/>
+      <c r="AC87" s="2"/>
+      <c r="AD87" s="2"/>
+      <c r="AE87" s="2"/>
+    </row>
+    <row r="88" spans="1:31">
       <c r="A88" s="3" t="s">
         <v>198</v>
       </c>
@@ -4685,6 +5448,12 @@
       <c r="E88" t="b">
         <v>1</v>
       </c>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+      <c r="K88" s="2"/>
       <c r="L88" t="s">
         <v>168</v>
       </c>
@@ -4715,8 +5484,14 @@
       <c r="U88" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="89" spans="1:21">
+      <c r="Z88" s="2"/>
+      <c r="AA88" s="2"/>
+      <c r="AB88" s="2"/>
+      <c r="AC88" s="2"/>
+      <c r="AD88" s="2"/>
+      <c r="AE88" s="2"/>
+    </row>
+    <row r="89" spans="1:31">
       <c r="A89" s="3" t="s">
         <v>199</v>
       </c>
@@ -4726,6 +5501,12 @@
       <c r="E89" t="b">
         <v>1</v>
       </c>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
       <c r="L89" t="s">
         <v>172</v>
       </c>
@@ -4756,8 +5537,14 @@
       <c r="U89" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="90" spans="1:21">
+      <c r="Z89" s="2"/>
+      <c r="AA89" s="2"/>
+      <c r="AB89" s="2"/>
+      <c r="AC89" s="2"/>
+      <c r="AD89" s="2"/>
+      <c r="AE89" s="2"/>
+    </row>
+    <row r="90" spans="1:31">
       <c r="A90" s="3" t="s">
         <v>200</v>
       </c>
@@ -4770,6 +5557,12 @@
       <c r="E90" t="b">
         <v>1</v>
       </c>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
       <c r="L90" t="s">
         <v>170</v>
       </c>
@@ -4800,8 +5593,14 @@
       <c r="U90" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="91" spans="1:21">
+      <c r="Z90" s="2"/>
+      <c r="AA90" s="2"/>
+      <c r="AB90" s="2"/>
+      <c r="AC90" s="2"/>
+      <c r="AD90" s="2"/>
+      <c r="AE90" s="2"/>
+    </row>
+    <row r="91" spans="1:31">
       <c r="A91" s="3" t="s">
         <v>202</v>
       </c>
@@ -4811,6 +5610,12 @@
       <c r="E91" t="b">
         <v>1</v>
       </c>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
       <c r="L91" t="s">
         <v>169</v>
       </c>
@@ -4841,8 +5646,14 @@
       <c r="U91" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="92" spans="1:21">
+      <c r="Z91" s="2"/>
+      <c r="AA91" s="2"/>
+      <c r="AB91" s="2"/>
+      <c r="AC91" s="2"/>
+      <c r="AD91" s="2"/>
+      <c r="AE91" s="2"/>
+    </row>
+    <row r="92" spans="1:31">
       <c r="A92" s="3" t="s">
         <v>203</v>
       </c>
@@ -4852,6 +5663,12 @@
       <c r="E92" t="b">
         <v>1</v>
       </c>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
       <c r="L92" t="s">
         <v>170</v>
       </c>
@@ -4882,8 +5699,14 @@
       <c r="U92" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="93" spans="1:21">
+      <c r="Z92" s="2"/>
+      <c r="AA92" s="2"/>
+      <c r="AB92" s="2"/>
+      <c r="AC92" s="2"/>
+      <c r="AD92" s="2"/>
+      <c r="AE92" s="2"/>
+    </row>
+    <row r="93" spans="1:31">
       <c r="A93" s="3" t="s">
         <v>204</v>
       </c>
@@ -4893,6 +5716,12 @@
       <c r="E93" t="b">
         <v>1</v>
       </c>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
       <c r="L93" t="s">
         <v>169</v>
       </c>
@@ -4923,8 +5752,14 @@
       <c r="U93" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="94" spans="1:21">
+      <c r="Z93" s="2"/>
+      <c r="AA93" s="2"/>
+      <c r="AB93" s="2"/>
+      <c r="AC93" s="2"/>
+      <c r="AD93" s="2"/>
+      <c r="AE93" s="2"/>
+    </row>
+    <row r="94" spans="1:31">
       <c r="A94" s="3" t="s">
         <v>205</v>
       </c>
@@ -4934,8 +5769,20 @@
       <c r="E94" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:21">
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+      <c r="Z94" s="2"/>
+      <c r="AA94" s="2"/>
+      <c r="AB94" s="2"/>
+      <c r="AC94" s="2"/>
+      <c r="AD94" s="2"/>
+      <c r="AE94" s="2"/>
+    </row>
+    <row r="95" spans="1:31">
       <c r="A95" s="3" t="s">
         <v>206</v>
       </c>
@@ -4945,8 +5792,20 @@
       <c r="E95" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:21">
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+      <c r="Z95" s="2"/>
+      <c r="AA95" s="2"/>
+      <c r="AB95" s="2"/>
+      <c r="AC95" s="2"/>
+      <c r="AD95" s="2"/>
+      <c r="AE95" s="2"/>
+    </row>
+    <row r="96" spans="1:31">
       <c r="A96" s="3" t="s">
         <v>207</v>
       </c>
@@ -4956,8 +5815,20 @@
       <c r="E96" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+      <c r="Z96" s="2"/>
+      <c r="AA96" s="2"/>
+      <c r="AB96" s="2"/>
+      <c r="AC96" s="2"/>
+      <c r="AD96" s="2"/>
+      <c r="AE96" s="2"/>
+    </row>
+    <row r="97" spans="1:31">
       <c r="A97" s="3" t="s">
         <v>208</v>
       </c>
@@ -4967,8 +5838,20 @@
       <c r="E97" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="Z97" s="2"/>
+      <c r="AA97" s="2"/>
+      <c r="AB97" s="2"/>
+      <c r="AC97" s="2"/>
+      <c r="AD97" s="2"/>
+      <c r="AE97" s="2"/>
+    </row>
+    <row r="98" spans="1:31">
       <c r="A98" s="3" t="s">
         <v>209</v>
       </c>
@@ -4978,8 +5861,20 @@
       <c r="E98" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
+      <c r="Z98" s="2"/>
+      <c r="AA98" s="2"/>
+      <c r="AB98" s="2"/>
+      <c r="AC98" s="2"/>
+      <c r="AD98" s="2"/>
+      <c r="AE98" s="2"/>
+    </row>
+    <row r="99" spans="1:31">
       <c r="A99" s="3" t="s">
         <v>210</v>
       </c>
@@ -4989,8 +5884,20 @@
       <c r="E99" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+      <c r="Z99" s="2"/>
+      <c r="AA99" s="2"/>
+      <c r="AB99" s="2"/>
+      <c r="AC99" s="2"/>
+      <c r="AD99" s="2"/>
+      <c r="AE99" s="2"/>
+    </row>
+    <row r="100" spans="1:31">
       <c r="A100" s="3" t="s">
         <v>211</v>
       </c>
@@ -5000,8 +5907,20 @@
       <c r="E100" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+      <c r="Z100" s="2"/>
+      <c r="AA100" s="2"/>
+      <c r="AB100" s="2"/>
+      <c r="AC100" s="2"/>
+      <c r="AD100" s="2"/>
+      <c r="AE100" s="2"/>
+    </row>
+    <row r="101" spans="1:31">
       <c r="A101" s="3" t="s">
         <v>212</v>
       </c>
@@ -5011,8 +5930,20 @@
       <c r="E101" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="Z101" s="2"/>
+      <c r="AA101" s="2"/>
+      <c r="AB101" s="2"/>
+      <c r="AC101" s="2"/>
+      <c r="AD101" s="2"/>
+      <c r="AE101" s="2"/>
+    </row>
+    <row r="102" spans="1:31">
       <c r="A102" s="3" t="s">
         <v>213</v>
       </c>
@@ -5022,8 +5953,20 @@
       <c r="E102" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="Z102" s="2"/>
+      <c r="AA102" s="2"/>
+      <c r="AB102" s="2"/>
+      <c r="AC102" s="2"/>
+      <c r="AD102" s="2"/>
+      <c r="AE102" s="2"/>
+    </row>
+    <row r="103" spans="1:31">
       <c r="A103" s="3" t="s">
         <v>214</v>
       </c>
@@ -5033,8 +5976,20 @@
       <c r="E103" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+      <c r="Z103" s="2"/>
+      <c r="AA103" s="2"/>
+      <c r="AB103" s="2"/>
+      <c r="AC103" s="2"/>
+      <c r="AD103" s="2"/>
+      <c r="AE103" s="2"/>
+    </row>
+    <row r="104" spans="1:31">
       <c r="A104" s="3" t="s">
         <v>215</v>
       </c>
@@ -5044,8 +5999,20 @@
       <c r="E104" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+      <c r="Z104" s="2"/>
+      <c r="AA104" s="2"/>
+      <c r="AB104" s="2"/>
+      <c r="AC104" s="2"/>
+      <c r="AD104" s="2"/>
+      <c r="AE104" s="2"/>
+    </row>
+    <row r="105" spans="1:31">
       <c r="A105" s="3" t="s">
         <v>216</v>
       </c>
@@ -5055,8 +6022,20 @@
       <c r="E105" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+      <c r="Z105" s="2"/>
+      <c r="AA105" s="2"/>
+      <c r="AB105" s="2"/>
+      <c r="AC105" s="2"/>
+      <c r="AD105" s="2"/>
+      <c r="AE105" s="2"/>
+    </row>
+    <row r="106" spans="1:31">
       <c r="A106" s="3" t="s">
         <v>217</v>
       </c>
@@ -5066,8 +6045,20 @@
       <c r="E106" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+      <c r="Z106" s="2"/>
+      <c r="AA106" s="2"/>
+      <c r="AB106" s="2"/>
+      <c r="AC106" s="2"/>
+      <c r="AD106" s="2"/>
+      <c r="AE106" s="2"/>
+    </row>
+    <row r="107" spans="1:31">
       <c r="A107" s="3" t="s">
         <v>218</v>
       </c>
@@ -5077,8 +6068,20 @@
       <c r="E107" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+      <c r="Z107" s="2"/>
+      <c r="AA107" s="2"/>
+      <c r="AB107" s="2"/>
+      <c r="AC107" s="2"/>
+      <c r="AD107" s="2"/>
+      <c r="AE107" s="2"/>
+    </row>
+    <row r="108" spans="1:31">
       <c r="A108" s="3" t="s">
         <v>219</v>
       </c>
@@ -5088,8 +6091,20 @@
       <c r="E108" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+      <c r="Z108" s="2"/>
+      <c r="AA108" s="2"/>
+      <c r="AB108" s="2"/>
+      <c r="AC108" s="2"/>
+      <c r="AD108" s="2"/>
+      <c r="AE108" s="2"/>
+    </row>
+    <row r="109" spans="1:31">
       <c r="A109" s="3" t="s">
         <v>221</v>
       </c>
@@ -5099,8 +6114,20 @@
       <c r="E109" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="Z109" s="2"/>
+      <c r="AA109" s="2"/>
+      <c r="AB109" s="2"/>
+      <c r="AC109" s="2"/>
+      <c r="AD109" s="2"/>
+      <c r="AE109" s="2"/>
+    </row>
+    <row r="110" spans="1:31">
       <c r="A110" s="3" t="s">
         <v>222</v>
       </c>
@@ -5110,8 +6137,20 @@
       <c r="E110" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+      <c r="Z110" s="2"/>
+      <c r="AA110" s="2"/>
+      <c r="AB110" s="2"/>
+      <c r="AC110" s="2"/>
+      <c r="AD110" s="2"/>
+      <c r="AE110" s="2"/>
+    </row>
+    <row r="111" spans="1:31">
       <c r="A111" s="3" t="s">
         <v>223</v>
       </c>
@@ -5121,8 +6160,20 @@
       <c r="E111" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+      <c r="Z111" s="2"/>
+      <c r="AA111" s="2"/>
+      <c r="AB111" s="2"/>
+      <c r="AC111" s="2"/>
+      <c r="AD111" s="2"/>
+      <c r="AE111" s="2"/>
+    </row>
+    <row r="112" spans="1:31">
       <c r="A112" s="3" t="s">
         <v>224</v>
       </c>
@@ -5132,8 +6183,20 @@
       <c r="E112" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:19">
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+      <c r="Z112" s="2"/>
+      <c r="AA112" s="2"/>
+      <c r="AB112" s="2"/>
+      <c r="AC112" s="2"/>
+      <c r="AD112" s="2"/>
+      <c r="AE112" s="2"/>
+    </row>
+    <row r="113" spans="1:31">
       <c r="A113" s="3" t="s">
         <v>225</v>
       </c>
@@ -5143,8 +6206,20 @@
       <c r="E113" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:19">
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="Z113" s="2"/>
+      <c r="AA113" s="2"/>
+      <c r="AB113" s="2"/>
+      <c r="AC113" s="2"/>
+      <c r="AD113" s="2"/>
+      <c r="AE113" s="2"/>
+    </row>
+    <row r="114" spans="1:31">
       <c r="A114" s="3" t="s">
         <v>226</v>
       </c>
@@ -5154,8 +6229,20 @@
       <c r="E114" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:19">
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="Z114" s="2"/>
+      <c r="AA114" s="2"/>
+      <c r="AB114" s="2"/>
+      <c r="AC114" s="2"/>
+      <c r="AD114" s="2"/>
+      <c r="AE114" s="2"/>
+    </row>
+    <row r="115" spans="1:31">
       <c r="A115" s="3" t="s">
         <v>227</v>
       </c>
@@ -5165,8 +6252,20 @@
       <c r="E115" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:19">
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+      <c r="Z115" s="2"/>
+      <c r="AA115" s="2"/>
+      <c r="AB115" s="2"/>
+      <c r="AC115" s="2"/>
+      <c r="AD115" s="2"/>
+      <c r="AE115" s="2"/>
+    </row>
+    <row r="116" spans="1:31">
       <c r="A116" t="s">
         <v>236</v>
       </c>
@@ -5179,6 +6278,12 @@
       <c r="E116" t="b">
         <v>1</v>
       </c>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
       <c r="L116" t="s">
         <v>166</v>
       </c>
@@ -5203,8 +6308,14 @@
       <c r="S116" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="117" spans="1:19">
+      <c r="Z116" s="2"/>
+      <c r="AA116" s="2"/>
+      <c r="AB116" s="2"/>
+      <c r="AC116" s="2"/>
+      <c r="AD116" s="2"/>
+      <c r="AE116" s="2"/>
+    </row>
+    <row r="117" spans="1:31">
       <c r="A117" t="s">
         <v>238</v>
       </c>
@@ -5214,8 +6325,20 @@
       <c r="E117" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:19">
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+      <c r="Z117" s="2"/>
+      <c r="AA117" s="2"/>
+      <c r="AB117" s="2"/>
+      <c r="AC117" s="2"/>
+      <c r="AD117" s="2"/>
+      <c r="AE117" s="2"/>
+    </row>
+    <row r="118" spans="1:31">
       <c r="A118" t="s">
         <v>239</v>
       </c>
@@ -5228,8 +6351,20 @@
       <c r="E118" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:19">
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+      <c r="Z118" s="2"/>
+      <c r="AA118" s="2"/>
+      <c r="AB118" s="2"/>
+      <c r="AC118" s="2"/>
+      <c r="AD118" s="2"/>
+      <c r="AE118" s="2"/>
+    </row>
+    <row r="119" spans="1:31">
       <c r="A119" t="s">
         <v>241</v>
       </c>
@@ -5242,8 +6377,20 @@
       <c r="E119" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:19">
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+      <c r="Z119" s="2"/>
+      <c r="AA119" s="2"/>
+      <c r="AB119" s="2"/>
+      <c r="AC119" s="2"/>
+      <c r="AD119" s="2"/>
+      <c r="AE119" s="2"/>
+    </row>
+    <row r="120" spans="1:31">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -5253,8 +6400,20 @@
       <c r="E120" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:19">
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+      <c r="Z120" s="2"/>
+      <c r="AA120" s="2"/>
+      <c r="AB120" s="2"/>
+      <c r="AC120" s="2"/>
+      <c r="AD120" s="2"/>
+      <c r="AE120" s="2"/>
+    </row>
+    <row r="121" spans="1:31">
       <c r="A121" t="s">
         <v>243</v>
       </c>
@@ -5264,8 +6423,20 @@
       <c r="E121" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:19">
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+      <c r="Z121" s="2"/>
+      <c r="AA121" s="2"/>
+      <c r="AB121" s="2"/>
+      <c r="AC121" s="2"/>
+      <c r="AD121" s="2"/>
+      <c r="AE121" s="2"/>
+    </row>
+    <row r="122" spans="1:31">
       <c r="A122" t="s">
         <v>244</v>
       </c>
@@ -5278,8 +6449,20 @@
       <c r="E122" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:19">
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="Z122" s="2"/>
+      <c r="AA122" s="2"/>
+      <c r="AB122" s="2"/>
+      <c r="AC122" s="2"/>
+      <c r="AD122" s="2"/>
+      <c r="AE122" s="2"/>
+    </row>
+    <row r="123" spans="1:31">
       <c r="A123" t="s">
         <v>246</v>
       </c>
@@ -5292,8 +6475,20 @@
       <c r="E123" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:19">
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="Z123" s="2"/>
+      <c r="AA123" s="2"/>
+      <c r="AB123" s="2"/>
+      <c r="AC123" s="2"/>
+      <c r="AD123" s="2"/>
+      <c r="AE123" s="2"/>
+    </row>
+    <row r="124" spans="1:31">
       <c r="A124" t="s">
         <v>248</v>
       </c>
@@ -5306,8 +6501,20 @@
       <c r="E124" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:19">
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="Z124" s="2"/>
+      <c r="AA124" s="2"/>
+      <c r="AB124" s="2"/>
+      <c r="AC124" s="2"/>
+      <c r="AD124" s="2"/>
+      <c r="AE124" s="2"/>
+    </row>
+    <row r="125" spans="1:31">
       <c r="A125" t="s">
         <v>249</v>
       </c>
@@ -5317,8 +6524,20 @@
       <c r="E125" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:19">
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="Z125" s="2"/>
+      <c r="AA125" s="2"/>
+      <c r="AB125" s="2"/>
+      <c r="AC125" s="2"/>
+      <c r="AD125" s="2"/>
+      <c r="AE125" s="2"/>
+    </row>
+    <row r="126" spans="1:31">
       <c r="A126" t="s">
         <v>250</v>
       </c>
@@ -5328,8 +6547,20 @@
       <c r="E126" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:19">
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2"/>
+      <c r="K126" s="2"/>
+      <c r="Z126" s="2"/>
+      <c r="AA126" s="2"/>
+      <c r="AB126" s="2"/>
+      <c r="AC126" s="2"/>
+      <c r="AD126" s="2"/>
+      <c r="AE126" s="2"/>
+    </row>
+    <row r="127" spans="1:31">
       <c r="A127" t="s">
         <v>251</v>
       </c>
@@ -5339,8 +6570,20 @@
       <c r="E127" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:19">
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+      <c r="Z127" s="2"/>
+      <c r="AA127" s="2"/>
+      <c r="AB127" s="2"/>
+      <c r="AC127" s="2"/>
+      <c r="AD127" s="2"/>
+      <c r="AE127" s="2"/>
+    </row>
+    <row r="128" spans="1:31">
       <c r="A128" t="s">
         <v>252</v>
       </c>
@@ -5350,8 +6593,20 @@
       <c r="E128" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+      <c r="Z128" s="2"/>
+      <c r="AA128" s="2"/>
+      <c r="AB128" s="2"/>
+      <c r="AC128" s="2"/>
+      <c r="AD128" s="2"/>
+      <c r="AE128" s="2"/>
+    </row>
+    <row r="129" spans="1:31">
       <c r="A129" t="s">
         <v>253</v>
       </c>
@@ -5361,8 +6616,20 @@
       <c r="E129" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+      <c r="J129" s="2"/>
+      <c r="K129" s="2"/>
+      <c r="Z129" s="2"/>
+      <c r="AA129" s="2"/>
+      <c r="AB129" s="2"/>
+      <c r="AC129" s="2"/>
+      <c r="AD129" s="2"/>
+      <c r="AE129" s="2"/>
+    </row>
+    <row r="130" spans="1:31">
       <c r="A130" t="s">
         <v>254</v>
       </c>
@@ -5372,8 +6639,20 @@
       <c r="E130" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+      <c r="J130" s="2"/>
+      <c r="K130" s="2"/>
+      <c r="Z130" s="2"/>
+      <c r="AA130" s="2"/>
+      <c r="AB130" s="2"/>
+      <c r="AC130" s="2"/>
+      <c r="AD130" s="2"/>
+      <c r="AE130" s="2"/>
+    </row>
+    <row r="131" spans="1:31">
       <c r="A131" t="s">
         <v>255</v>
       </c>
@@ -5386,8 +6665,20 @@
       <c r="E131" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
+      <c r="Z131" s="2"/>
+      <c r="AA131" s="2"/>
+      <c r="AB131" s="2"/>
+      <c r="AC131" s="2"/>
+      <c r="AD131" s="2"/>
+      <c r="AE131" s="2"/>
+    </row>
+    <row r="132" spans="1:31">
       <c r="A132" t="s">
         <v>256</v>
       </c>
@@ -5397,8 +6688,20 @@
       <c r="E132" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="2"/>
+      <c r="I132" s="2"/>
+      <c r="J132" s="2"/>
+      <c r="K132" s="2"/>
+      <c r="Z132" s="2"/>
+      <c r="AA132" s="2"/>
+      <c r="AB132" s="2"/>
+      <c r="AC132" s="2"/>
+      <c r="AD132" s="2"/>
+      <c r="AE132" s="2"/>
+    </row>
+    <row r="133" spans="1:31">
       <c r="A133" t="s">
         <v>257</v>
       </c>
@@ -5408,8 +6711,20 @@
       <c r="E133" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2"/>
+      <c r="K133" s="2"/>
+      <c r="Z133" s="2"/>
+      <c r="AA133" s="2"/>
+      <c r="AB133" s="2"/>
+      <c r="AC133" s="2"/>
+      <c r="AD133" s="2"/>
+      <c r="AE133" s="2"/>
+    </row>
+    <row r="134" spans="1:31">
       <c r="A134" t="s">
         <v>258</v>
       </c>
@@ -5422,8 +6737,20 @@
       <c r="E134" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+      <c r="J134" s="2"/>
+      <c r="K134" s="2"/>
+      <c r="Z134" s="2"/>
+      <c r="AA134" s="2"/>
+      <c r="AB134" s="2"/>
+      <c r="AC134" s="2"/>
+      <c r="AD134" s="2"/>
+      <c r="AE134" s="2"/>
+    </row>
+    <row r="135" spans="1:31">
       <c r="A135" t="s">
         <v>259</v>
       </c>
@@ -5433,8 +6760,20 @@
       <c r="E135" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="2"/>
+      <c r="I135" s="2"/>
+      <c r="J135" s="2"/>
+      <c r="K135" s="2"/>
+      <c r="Z135" s="2"/>
+      <c r="AA135" s="2"/>
+      <c r="AB135" s="2"/>
+      <c r="AC135" s="2"/>
+      <c r="AD135" s="2"/>
+      <c r="AE135" s="2"/>
+    </row>
+    <row r="136" spans="1:31">
       <c r="A136" s="3" t="s">
         <v>260</v>
       </c>
@@ -5447,8 +6786,20 @@
       <c r="E136" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+      <c r="J136" s="2"/>
+      <c r="K136" s="2"/>
+      <c r="Z136" s="2"/>
+      <c r="AA136" s="2"/>
+      <c r="AB136" s="2"/>
+      <c r="AC136" s="2"/>
+      <c r="AD136" s="2"/>
+      <c r="AE136" s="2"/>
+    </row>
+    <row r="137" spans="1:31">
       <c r="A137" s="3" t="s">
         <v>261</v>
       </c>
@@ -5458,8 +6809,20 @@
       <c r="E137" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+      <c r="J137" s="2"/>
+      <c r="K137" s="2"/>
+      <c r="Z137" s="2"/>
+      <c r="AA137" s="2"/>
+      <c r="AB137" s="2"/>
+      <c r="AC137" s="2"/>
+      <c r="AD137" s="2"/>
+      <c r="AE137" s="2"/>
+    </row>
+    <row r="138" spans="1:31">
       <c r="A138" s="3" t="s">
         <v>262</v>
       </c>
@@ -5472,8 +6835,20 @@
       <c r="E138" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+      <c r="J138" s="2"/>
+      <c r="K138" s="2"/>
+      <c r="Z138" s="2"/>
+      <c r="AA138" s="2"/>
+      <c r="AB138" s="2"/>
+      <c r="AC138" s="2"/>
+      <c r="AD138" s="2"/>
+      <c r="AE138" s="2"/>
+    </row>
+    <row r="139" spans="1:31">
       <c r="A139" s="3" t="s">
         <v>263</v>
       </c>
@@ -5483,8 +6858,20 @@
       <c r="E139" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+      <c r="J139" s="2"/>
+      <c r="K139" s="2"/>
+      <c r="Z139" s="2"/>
+      <c r="AA139" s="2"/>
+      <c r="AB139" s="2"/>
+      <c r="AC139" s="2"/>
+      <c r="AD139" s="2"/>
+      <c r="AE139" s="2"/>
+    </row>
+    <row r="140" spans="1:31">
       <c r="A140" s="3" t="s">
         <v>264</v>
       </c>
@@ -5494,8 +6881,20 @@
       <c r="E140" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+      <c r="Z140" s="2"/>
+      <c r="AA140" s="2"/>
+      <c r="AB140" s="2"/>
+      <c r="AC140" s="2"/>
+      <c r="AD140" s="2"/>
+      <c r="AE140" s="2"/>
+    </row>
+    <row r="141" spans="1:31">
       <c r="A141" s="3" t="s">
         <v>265</v>
       </c>
@@ -5508,8 +6907,20 @@
       <c r="E141" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+      <c r="Z141" s="2"/>
+      <c r="AA141" s="2"/>
+      <c r="AB141" s="2"/>
+      <c r="AC141" s="2"/>
+      <c r="AD141" s="2"/>
+      <c r="AE141" s="2"/>
+    </row>
+    <row r="142" spans="1:31">
       <c r="A142" s="3" t="s">
         <v>266</v>
       </c>
@@ -5519,8 +6930,20 @@
       <c r="E142" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2"/>
+      <c r="K142" s="2"/>
+      <c r="Z142" s="2"/>
+      <c r="AA142" s="2"/>
+      <c r="AB142" s="2"/>
+      <c r="AC142" s="2"/>
+      <c r="AD142" s="2"/>
+      <c r="AE142" s="2"/>
+    </row>
+    <row r="143" spans="1:31">
       <c r="A143" s="3" t="s">
         <v>267</v>
       </c>
@@ -5530,8 +6953,20 @@
       <c r="E143" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+      <c r="H143" s="2"/>
+      <c r="I143" s="2"/>
+      <c r="J143" s="2"/>
+      <c r="K143" s="2"/>
+      <c r="Z143" s="2"/>
+      <c r="AA143" s="2"/>
+      <c r="AB143" s="2"/>
+      <c r="AC143" s="2"/>
+      <c r="AD143" s="2"/>
+      <c r="AE143" s="2"/>
+    </row>
+    <row r="144" spans="1:31">
       <c r="A144" s="3" t="s">
         <v>268</v>
       </c>
@@ -5541,8 +6976,20 @@
       <c r="E144" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+      <c r="J144" s="2"/>
+      <c r="K144" s="2"/>
+      <c r="Z144" s="2"/>
+      <c r="AA144" s="2"/>
+      <c r="AB144" s="2"/>
+      <c r="AC144" s="2"/>
+      <c r="AD144" s="2"/>
+      <c r="AE144" s="2"/>
+    </row>
+    <row r="145" spans="1:31">
       <c r="A145" s="3" t="s">
         <v>269</v>
       </c>
@@ -5552,8 +6999,20 @@
       <c r="E145" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+      <c r="Z145" s="2"/>
+      <c r="AA145" s="2"/>
+      <c r="AB145" s="2"/>
+      <c r="AC145" s="2"/>
+      <c r="AD145" s="2"/>
+      <c r="AE145" s="2"/>
+    </row>
+    <row r="146" spans="1:31">
       <c r="A146" s="3" t="s">
         <v>270</v>
       </c>
@@ -5563,8 +7022,20 @@
       <c r="E146" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2"/>
+      <c r="K146" s="2"/>
+      <c r="Z146" s="2"/>
+      <c r="AA146" s="2"/>
+      <c r="AB146" s="2"/>
+      <c r="AC146" s="2"/>
+      <c r="AD146" s="2"/>
+      <c r="AE146" s="2"/>
+    </row>
+    <row r="147" spans="1:31">
       <c r="A147" s="3" t="s">
         <v>271</v>
       </c>
@@ -5577,8 +7048,20 @@
       <c r="E147" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+      <c r="J147" s="2"/>
+      <c r="K147" s="2"/>
+      <c r="Z147" s="2"/>
+      <c r="AA147" s="2"/>
+      <c r="AB147" s="2"/>
+      <c r="AC147" s="2"/>
+      <c r="AD147" s="2"/>
+      <c r="AE147" s="2"/>
+    </row>
+    <row r="148" spans="1:31">
       <c r="A148" s="3" t="s">
         <v>272</v>
       </c>
@@ -5588,8 +7071,20 @@
       <c r="E148" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:5">
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+      <c r="J148" s="2"/>
+      <c r="K148" s="2"/>
+      <c r="Z148" s="2"/>
+      <c r="AA148" s="2"/>
+      <c r="AB148" s="2"/>
+      <c r="AC148" s="2"/>
+      <c r="AD148" s="2"/>
+      <c r="AE148" s="2"/>
+    </row>
+    <row r="149" spans="1:31">
       <c r="A149" s="3" t="s">
         <v>273</v>
       </c>
@@ -5602,8 +7097,20 @@
       <c r="E149" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+      <c r="H149" s="2"/>
+      <c r="I149" s="2"/>
+      <c r="J149" s="2"/>
+      <c r="K149" s="2"/>
+      <c r="Z149" s="2"/>
+      <c r="AA149" s="2"/>
+      <c r="AB149" s="2"/>
+      <c r="AC149" s="2"/>
+      <c r="AD149" s="2"/>
+      <c r="AE149" s="2"/>
+    </row>
+    <row r="150" spans="1:31">
       <c r="A150" s="3" t="s">
         <v>274</v>
       </c>
@@ -5613,8 +7120,20 @@
       <c r="E150" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+      <c r="H150" s="2"/>
+      <c r="I150" s="2"/>
+      <c r="J150" s="2"/>
+      <c r="K150" s="2"/>
+      <c r="Z150" s="2"/>
+      <c r="AA150" s="2"/>
+      <c r="AB150" s="2"/>
+      <c r="AC150" s="2"/>
+      <c r="AD150" s="2"/>
+      <c r="AE150" s="2"/>
+    </row>
+    <row r="151" spans="1:31">
       <c r="A151" s="3" t="s">
         <v>275</v>
       </c>
@@ -5624,8 +7143,20 @@
       <c r="E151" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+      <c r="H151" s="2"/>
+      <c r="I151" s="2"/>
+      <c r="J151" s="2"/>
+      <c r="K151" s="2"/>
+      <c r="Z151" s="2"/>
+      <c r="AA151" s="2"/>
+      <c r="AB151" s="2"/>
+      <c r="AC151" s="2"/>
+      <c r="AD151" s="2"/>
+      <c r="AE151" s="2"/>
+    </row>
+    <row r="152" spans="1:31">
       <c r="A152" s="3" t="s">
         <v>276</v>
       </c>
@@ -5635,8 +7166,20 @@
       <c r="E152" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+      <c r="J152" s="2"/>
+      <c r="K152" s="2"/>
+      <c r="Z152" s="2"/>
+      <c r="AA152" s="2"/>
+      <c r="AB152" s="2"/>
+      <c r="AC152" s="2"/>
+      <c r="AD152" s="2"/>
+      <c r="AE152" s="2"/>
+    </row>
+    <row r="153" spans="1:31">
       <c r="A153" s="3" t="s">
         <v>277</v>
       </c>
@@ -5646,8 +7189,20 @@
       <c r="E153" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+      <c r="H153" s="2"/>
+      <c r="I153" s="2"/>
+      <c r="J153" s="2"/>
+      <c r="K153" s="2"/>
+      <c r="Z153" s="2"/>
+      <c r="AA153" s="2"/>
+      <c r="AB153" s="2"/>
+      <c r="AC153" s="2"/>
+      <c r="AD153" s="2"/>
+      <c r="AE153" s="2"/>
+    </row>
+    <row r="154" spans="1:31">
       <c r="A154" s="3" t="s">
         <v>278</v>
       </c>
@@ -5657,8 +7212,20 @@
       <c r="E154" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2"/>
+      <c r="K154" s="2"/>
+      <c r="Z154" s="2"/>
+      <c r="AA154" s="2"/>
+      <c r="AB154" s="2"/>
+      <c r="AC154" s="2"/>
+      <c r="AD154" s="2"/>
+      <c r="AE154" s="2"/>
+    </row>
+    <row r="155" spans="1:31">
       <c r="A155" s="3" t="s">
         <v>279</v>
       </c>
@@ -5668,8 +7235,20 @@
       <c r="E155" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
+      <c r="Z155" s="2"/>
+      <c r="AA155" s="2"/>
+      <c r="AB155" s="2"/>
+      <c r="AC155" s="2"/>
+      <c r="AD155" s="2"/>
+      <c r="AE155" s="2"/>
+    </row>
+    <row r="156" spans="1:31">
       <c r="A156" s="3" t="s">
         <v>280</v>
       </c>
@@ -5679,8 +7258,20 @@
       <c r="E156" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+      <c r="H156" s="2"/>
+      <c r="I156" s="2"/>
+      <c r="J156" s="2"/>
+      <c r="K156" s="2"/>
+      <c r="Z156" s="2"/>
+      <c r="AA156" s="2"/>
+      <c r="AB156" s="2"/>
+      <c r="AC156" s="2"/>
+      <c r="AD156" s="2"/>
+      <c r="AE156" s="2"/>
+    </row>
+    <row r="157" spans="1:31">
       <c r="A157" s="3" t="s">
         <v>281</v>
       </c>
@@ -5690,8 +7281,20 @@
       <c r="E157" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+      <c r="H157" s="2"/>
+      <c r="I157" s="2"/>
+      <c r="J157" s="2"/>
+      <c r="K157" s="2"/>
+      <c r="Z157" s="2"/>
+      <c r="AA157" s="2"/>
+      <c r="AB157" s="2"/>
+      <c r="AC157" s="2"/>
+      <c r="AD157" s="2"/>
+      <c r="AE157" s="2"/>
+    </row>
+    <row r="158" spans="1:31">
       <c r="A158" s="3" t="s">
         <v>282</v>
       </c>
@@ -5704,6 +7307,145 @@
       <c r="E158" t="b">
         <v>1</v>
       </c>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="H158" s="2"/>
+      <c r="I158" s="2"/>
+      <c r="J158" s="2"/>
+      <c r="K158" s="2"/>
+      <c r="Z158" s="2"/>
+      <c r="AA158" s="2"/>
+      <c r="AB158" s="2"/>
+      <c r="AC158" s="2"/>
+      <c r="AD158" s="2"/>
+      <c r="AE158" s="2"/>
+    </row>
+    <row r="159" spans="1:31">
+      <c r="A159" t="s">
+        <v>284</v>
+      </c>
+      <c r="C159" t="s">
+        <v>154</v>
+      </c>
+      <c r="D159" t="s">
+        <v>283</v>
+      </c>
+      <c r="E159" t="b">
+        <v>1</v>
+      </c>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+      <c r="H159" s="2"/>
+      <c r="I159" s="2"/>
+      <c r="J159" s="2"/>
+      <c r="K159" s="2"/>
+      <c r="Z159" s="2"/>
+      <c r="AA159" s="2"/>
+      <c r="AB159" s="2"/>
+      <c r="AC159" s="2"/>
+      <c r="AD159" s="2"/>
+      <c r="AE159" s="2"/>
+    </row>
+    <row r="160" spans="1:31">
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2"/>
+      <c r="K160" s="2"/>
+      <c r="Z160" s="2"/>
+      <c r="AA160" s="2"/>
+      <c r="AB160" s="2"/>
+      <c r="AC160" s="2"/>
+      <c r="AD160" s="2"/>
+      <c r="AE160" s="2"/>
+    </row>
+    <row r="161" spans="6:31">
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+      <c r="J161" s="2"/>
+      <c r="K161" s="2"/>
+      <c r="Z161" s="2"/>
+      <c r="AA161" s="2"/>
+      <c r="AB161" s="2"/>
+      <c r="AC161" s="2"/>
+      <c r="AD161" s="2"/>
+      <c r="AE161" s="2"/>
+    </row>
+    <row r="162" spans="6:31">
+      <c r="F162" s="2"/>
+      <c r="G162" s="2"/>
+      <c r="H162" s="2"/>
+      <c r="I162" s="2"/>
+      <c r="J162" s="2"/>
+      <c r="K162" s="2"/>
+      <c r="Z162" s="2"/>
+      <c r="AA162" s="2"/>
+      <c r="AB162" s="2"/>
+      <c r="AC162" s="2"/>
+      <c r="AD162" s="2"/>
+      <c r="AE162" s="2"/>
+    </row>
+    <row r="163" spans="6:31">
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
+      <c r="H163" s="2"/>
+      <c r="I163" s="2"/>
+      <c r="J163" s="2"/>
+      <c r="K163" s="2"/>
+      <c r="Z163" s="2"/>
+      <c r="AA163" s="2"/>
+      <c r="AB163" s="2"/>
+      <c r="AC163" s="2"/>
+      <c r="AD163" s="2"/>
+      <c r="AE163" s="2"/>
+    </row>
+    <row r="164" spans="6:31">
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
+      <c r="H164" s="2"/>
+      <c r="I164" s="2"/>
+      <c r="J164" s="2"/>
+      <c r="K164" s="2"/>
+      <c r="Z164" s="2"/>
+      <c r="AA164" s="2"/>
+      <c r="AB164" s="2"/>
+      <c r="AC164" s="2"/>
+      <c r="AD164" s="2"/>
+      <c r="AE164" s="2"/>
+    </row>
+    <row r="165" spans="6:31">
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+      <c r="J165" s="2"/>
+      <c r="K165" s="2"/>
+      <c r="Z165" s="2"/>
+      <c r="AA165" s="2"/>
+      <c r="AB165" s="2"/>
+      <c r="AC165" s="2"/>
+      <c r="AD165" s="2"/>
+      <c r="AE165" s="2"/>
+    </row>
+    <row r="166" spans="6:31">
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="2"/>
+      <c r="I166" s="2"/>
+      <c r="J166" s="2"/>
+      <c r="K166" s="2"/>
+      <c r="Z166" s="2"/>
+      <c r="AA166" s="2"/>
+      <c r="AB166" s="2"/>
+      <c r="AC166" s="2"/>
+      <c r="AD166" s="2"/>
+      <c r="AE166" s="2"/>
+    </row>
+    <row r="167" spans="6:31">
+      <c r="F167" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>